<commit_message>
removed two overfull errors
</commit_message>
<xml_diff>
--- a/doc/SoftwareManagement/Projektplan.xlsx
+++ b/doc/SoftwareManagement/Projektplan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="22221"/>
-  <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <workbookPr codeName="ThisWorkbook" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="10820" windowHeight="10100" tabRatio="676" activeTab="1"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="10815" windowHeight="10095" tabRatio="676"/>
   </bookViews>
   <sheets>
     <sheet name="Details" sheetId="9" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="13" r:id="rId2"/>
+    <sheet name="Projektplan" sheetId="13" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="89">
   <si>
     <t>Task</t>
   </si>
@@ -172,9 +172,6 @@
     <t>Object Caching</t>
   </si>
   <si>
-    <t>Semesterarbeit</t>
-  </si>
-  <si>
     <t>Lukas Hofmaier</t>
   </si>
   <si>
@@ -284,6 +281,12 @@
   </si>
   <si>
     <t>Semesterdaten</t>
+  </si>
+  <si>
+    <t>Studienarbeit</t>
+  </si>
+  <si>
+    <t>Korrekturen am Zeitplan</t>
   </si>
 </sst>
 </file>
@@ -1045,85 +1048,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="22" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="22" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="21" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="21" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="13" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="21" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1140,28 +1093,78 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="21" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="21" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="13" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="21" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="22" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="22" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1539,24 +1542,24 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A3:F29"/>
+  <dimension ref="A3:F30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="25.33203125" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="29.83203125" customWidth="1"/>
-    <col min="5" max="5" width="16.5" customWidth="1"/>
-    <col min="6" max="6" width="40.1640625" customWidth="1"/>
+    <col min="4" max="4" width="29.85546875" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" customWidth="1"/>
+    <col min="6" max="6" width="40.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:6" ht="28">
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.4">
       <c r="A3" s="123" t="s">
-        <v>50</v>
+        <v>87</v>
       </c>
       <c r="B3" s="123"/>
       <c r="C3" s="123"/>
@@ -1564,7 +1567,7 @@
       <c r="E3" s="14"/>
       <c r="F3" s="14"/>
     </row>
-    <row r="4" spans="1:6" ht="12.75" customHeight="1">
+    <row r="4" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="12"/>
       <c r="B4" s="12"/>
       <c r="C4" s="12"/>
@@ -1572,7 +1575,7 @@
       <c r="E4" s="12"/>
       <c r="F4" s="12"/>
     </row>
-    <row r="5" spans="1:6" ht="31">
+    <row r="5" spans="1:6" ht="33.75" x14ac:dyDescent="0.5">
       <c r="A5" s="122" t="s">
         <v>49</v>
       </c>
@@ -1582,15 +1585,15 @@
       <c r="E5" s="13"/>
       <c r="F5" s="13"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="126"/>
       <c r="B6" s="127"/>
       <c r="C6" s="127"/>
       <c r="D6" s="127"/>
     </row>
-    <row r="7" spans="1:6" s="30" customFormat="1"/>
-    <row r="8" spans="1:6" ht="13" thickBot="1"/>
-    <row r="9" spans="1:6" ht="19" thickBot="1">
+    <row r="7" spans="1:6" s="30" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:6" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="52" t="s">
         <v>9</v>
       </c>
@@ -1602,27 +1605,27 @@
       </c>
       <c r="F9" s="124"/>
     </row>
-    <row r="10" spans="1:6" ht="18">
+    <row r="10" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
       <c r="B10" s="54" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C10" s="55" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E10" s="125">
         <v>40959</v>
       </c>
       <c r="F10" s="125"/>
     </row>
-    <row r="11" spans="1:6" ht="18">
+    <row r="11" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
       <c r="B11" s="56" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C11" s="57" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="19" thickBot="1">
+    <row r="12" spans="1:6" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="56" t="s">
         <v>29</v>
       </c>
@@ -1630,8 +1633,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="13" thickBot="1"/>
-    <row r="15" spans="1:6" ht="24">
+    <row r="14" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B15" s="31" t="s">
         <v>33</v>
       </c>
@@ -1639,10 +1642,10 @@
         <v>40959</v>
       </c>
       <c r="D15" s="33" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="13" thickBot="1">
+    <row r="16" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B16" s="34" t="s">
         <v>34</v>
       </c>
@@ -1650,15 +1653,15 @@
         <v>40959</v>
       </c>
       <c r="D16" s="36" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
-    <row r="18" spans="2:6" s="29" customFormat="1" ht="13" thickBot="1">
+    <row r="18" spans="2:6" s="29" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B18" s="37" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="2:6" s="29" customFormat="1">
+    <row r="19" spans="2:6" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B19" s="42" t="s">
         <v>36</v>
       </c>
@@ -1675,7 +1678,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="2:6" s="29" customFormat="1">
+    <row r="20" spans="2:6" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B20" s="38">
         <v>1</v>
       </c>
@@ -1683,7 +1686,7 @@
         <v>46</v>
       </c>
       <c r="D20" s="40">
-        <v>40965</v>
+        <v>40964</v>
       </c>
       <c r="E20" s="39" t="s">
         <v>30</v>
@@ -1692,7 +1695,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="2:6" s="29" customFormat="1">
+    <row r="21" spans="2:6" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B21" s="38">
         <v>1.1000000000000001</v>
       </c>
@@ -1700,7 +1703,7 @@
         <v>46</v>
       </c>
       <c r="D21" s="40">
-        <v>40970</v>
+        <v>40964</v>
       </c>
       <c r="E21" s="39" t="s">
         <v>30</v>
@@ -1709,30 +1712,47 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="2:6" s="29" customFormat="1" ht="13" thickBot="1">
-      <c r="B22" s="45">
+    <row r="22" spans="2:6" s="29" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="38">
         <v>1.2</v>
       </c>
-      <c r="C22" s="46" t="s">
+      <c r="C22" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="D22" s="65">
+      <c r="D22" s="40">
+        <v>40984</v>
+      </c>
+      <c r="E22" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="F22" s="41" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" s="29" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="45">
+        <v>1.3</v>
+      </c>
+      <c r="C23" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="D23" s="65">
         <v>41052</v>
       </c>
-      <c r="E22" s="111" t="s">
+      <c r="E23" s="111" t="s">
         <v>30</v>
       </c>
-      <c r="F22" s="112" t="s">
-        <v>84</v>
+      <c r="F23" s="112" t="s">
+        <v>83</v>
       </c>
     </row>
-    <row r="23" spans="2:6" s="29" customFormat="1"/>
-    <row r="24" spans="2:6" s="29" customFormat="1"/>
-    <row r="25" spans="2:6" s="29" customFormat="1"/>
-    <row r="26" spans="2:6" s="29" customFormat="1"/>
-    <row r="27" spans="2:6" s="29" customFormat="1"/>
-    <row r="28" spans="2:6" s="29" customFormat="1"/>
-    <row r="29" spans="2:6" s="29" customFormat="1"/>
+    <row r="24" spans="2:6" s="29" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="2:6" s="29" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="2:6" s="29" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="2:6" s="29" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="2:6" s="29" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="2:6" s="29" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="2:6" s="29" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A5:D5"/>
@@ -1757,45 +1777,45 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DO56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="A3" sqref="A3:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="41.83203125" style="69" customWidth="1"/>
-    <col min="2" max="2" width="6.33203125" style="69" customWidth="1"/>
-    <col min="3" max="12" width="4.5" style="69" customWidth="1"/>
-    <col min="13" max="14" width="5.6640625" style="69" bestFit="1" customWidth="1"/>
-    <col min="15" max="18" width="4.5" style="69" customWidth="1"/>
-    <col min="19" max="19" width="5.33203125" style="69" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.85546875" style="69" customWidth="1"/>
+    <col min="2" max="2" width="6.28515625" style="69" customWidth="1"/>
+    <col min="3" max="12" width="4.42578125" style="69" customWidth="1"/>
+    <col min="13" max="14" width="5.7109375" style="69" bestFit="1" customWidth="1"/>
+    <col min="15" max="18" width="4.42578125" style="69" customWidth="1"/>
+    <col min="19" max="19" width="5.28515625" style="69" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="6" style="69" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="5.6640625" style="69" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="4.5" style="69" customWidth="1"/>
-    <col min="24" max="24" width="4.83203125" style="69" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="4.83203125" style="69" customWidth="1"/>
-    <col min="26" max="26" width="4.5" style="6" customWidth="1"/>
-    <col min="27" max="27" width="5.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="28" max="30" width="4.5" style="6" customWidth="1"/>
+    <col min="21" max="21" width="5.7109375" style="69" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="4.42578125" style="69" customWidth="1"/>
+    <col min="24" max="24" width="4.85546875" style="69" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="4.85546875" style="69" customWidth="1"/>
+    <col min="26" max="26" width="4.42578125" style="6" customWidth="1"/>
+    <col min="27" max="27" width="5.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="28" max="30" width="4.42578125" style="6" customWidth="1"/>
     <col min="31" max="31" width="6" style="6" bestFit="1" customWidth="1"/>
-    <col min="32" max="36" width="4.5" style="6" customWidth="1"/>
+    <col min="32" max="36" width="4.42578125" style="6" customWidth="1"/>
     <col min="37" max="37" width="6" style="6" bestFit="1" customWidth="1"/>
-    <col min="38" max="42" width="4.5" style="6" customWidth="1"/>
+    <col min="38" max="42" width="4.42578125" style="6" customWidth="1"/>
     <col min="43" max="43" width="6" style="6" bestFit="1" customWidth="1"/>
-    <col min="44" max="92" width="4.5" style="6" customWidth="1"/>
-    <col min="93" max="112" width="4.6640625" style="6" customWidth="1"/>
-    <col min="113" max="113" width="4.5" style="6" customWidth="1"/>
-    <col min="114" max="16384" width="9.1640625" style="6"/>
+    <col min="44" max="92" width="4.42578125" style="6" customWidth="1"/>
+    <col min="93" max="112" width="4.7109375" style="6" customWidth="1"/>
+    <col min="113" max="113" width="4.42578125" style="6" customWidth="1"/>
+    <col min="114" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:119" ht="17">
+    <row r="1" spans="1:119" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B1" s="2"/>
     </row>
-    <row r="2" spans="1:119" ht="13.5" customHeight="1">
+    <row r="2" spans="1:119" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="8"/>
       <c r="B2" s="108"/>
       <c r="C2" s="64"/>
@@ -1807,117 +1827,117 @@
       <c r="CS2" s="64"/>
       <c r="CT2" s="64"/>
     </row>
-    <row r="3" spans="1:119" ht="13">
+    <row r="3" spans="1:119" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
-      <c r="C3" s="164" t="s">
+      <c r="C3" s="137" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="164"/>
-      <c r="E3" s="164"/>
-      <c r="F3" s="164"/>
-      <c r="G3" s="164"/>
-      <c r="H3" s="164"/>
-      <c r="I3" s="135" t="s">
-        <v>79</v>
-      </c>
-      <c r="J3" s="135"/>
-      <c r="K3" s="135"/>
-      <c r="L3" s="135"/>
-      <c r="M3" s="135"/>
-      <c r="N3" s="135"/>
-      <c r="O3" s="135"/>
-      <c r="P3" s="135"/>
-      <c r="Q3" s="135"/>
-      <c r="R3" s="135"/>
-      <c r="S3" s="135"/>
-      <c r="T3" s="135"/>
-      <c r="U3" s="135"/>
-      <c r="V3" s="135"/>
-      <c r="W3" s="136" t="s">
+      <c r="D3" s="137"/>
+      <c r="E3" s="137"/>
+      <c r="F3" s="137"/>
+      <c r="G3" s="137"/>
+      <c r="H3" s="137"/>
+      <c r="I3" s="145" t="s">
         <v>78</v>
       </c>
-      <c r="X3" s="136"/>
-      <c r="Y3" s="136"/>
-      <c r="Z3" s="136"/>
-      <c r="AA3" s="136"/>
-      <c r="AB3" s="136"/>
-      <c r="AC3" s="136"/>
-      <c r="AD3" s="136"/>
-      <c r="AE3" s="136"/>
-      <c r="AF3" s="136"/>
-      <c r="AG3" s="136"/>
-      <c r="AH3" s="136"/>
-      <c r="AI3" s="137" t="s">
+      <c r="J3" s="145"/>
+      <c r="K3" s="145"/>
+      <c r="L3" s="145"/>
+      <c r="M3" s="145"/>
+      <c r="N3" s="145"/>
+      <c r="O3" s="145"/>
+      <c r="P3" s="145"/>
+      <c r="Q3" s="145"/>
+      <c r="R3" s="145"/>
+      <c r="S3" s="145"/>
+      <c r="T3" s="145"/>
+      <c r="U3" s="145"/>
+      <c r="V3" s="145"/>
+      <c r="W3" s="146" t="s">
         <v>77</v>
       </c>
-      <c r="AJ3" s="137"/>
-      <c r="AK3" s="137"/>
-      <c r="AL3" s="137"/>
-      <c r="AM3" s="137"/>
-      <c r="AN3" s="137"/>
-      <c r="AO3" s="137"/>
-      <c r="AP3" s="137"/>
-      <c r="AQ3" s="137"/>
-      <c r="AR3" s="137"/>
-      <c r="AS3" s="137"/>
-      <c r="AT3" s="137"/>
-      <c r="AU3" s="137"/>
-      <c r="AV3" s="137"/>
-      <c r="AW3" s="137"/>
-      <c r="AX3" s="137"/>
-      <c r="AY3" s="137"/>
-      <c r="AZ3" s="137"/>
-      <c r="BA3" s="137"/>
-      <c r="BB3" s="137"/>
-      <c r="BC3" s="137"/>
-      <c r="BD3" s="137"/>
-      <c r="BE3" s="137"/>
-      <c r="BF3" s="137"/>
-      <c r="BG3" s="137"/>
-      <c r="BH3" s="137"/>
-      <c r="BI3" s="137"/>
-      <c r="BJ3" s="137"/>
-      <c r="BK3" s="137"/>
-      <c r="BL3" s="137"/>
-      <c r="BM3" s="137"/>
-      <c r="BN3" s="137"/>
-      <c r="BO3" s="137"/>
-      <c r="BP3" s="137"/>
-      <c r="BQ3" s="136" t="s">
+      <c r="X3" s="146"/>
+      <c r="Y3" s="146"/>
+      <c r="Z3" s="146"/>
+      <c r="AA3" s="146"/>
+      <c r="AB3" s="146"/>
+      <c r="AC3" s="146"/>
+      <c r="AD3" s="146"/>
+      <c r="AE3" s="146"/>
+      <c r="AF3" s="146"/>
+      <c r="AG3" s="146"/>
+      <c r="AH3" s="146"/>
+      <c r="AI3" s="136" t="s">
         <v>76</v>
       </c>
-      <c r="BR3" s="136"/>
-      <c r="BS3" s="136"/>
-      <c r="BT3" s="136"/>
-      <c r="BU3" s="136"/>
-      <c r="BV3" s="136"/>
-      <c r="BW3" s="136"/>
-      <c r="BX3" s="136"/>
-      <c r="BY3" s="136"/>
-      <c r="BZ3" s="136"/>
-      <c r="CA3" s="136"/>
-      <c r="CB3" s="136"/>
-      <c r="CC3" s="136"/>
-      <c r="CD3" s="136"/>
-      <c r="CE3" s="136"/>
-      <c r="CF3" s="136"/>
-      <c r="CG3" s="136"/>
-      <c r="CH3" s="136"/>
-      <c r="CI3" s="137" t="s">
-        <v>83</v>
-      </c>
-      <c r="CJ3" s="137"/>
-      <c r="CK3" s="137"/>
-      <c r="CL3" s="137"/>
-      <c r="CM3" s="137"/>
-      <c r="CN3" s="137"/>
-      <c r="CO3" s="137"/>
-      <c r="CP3" s="137"/>
-      <c r="CQ3" s="137"/>
-      <c r="CR3" s="137"/>
-      <c r="CS3" s="137"/>
-      <c r="CT3" s="137"/>
+      <c r="AJ3" s="136"/>
+      <c r="AK3" s="136"/>
+      <c r="AL3" s="136"/>
+      <c r="AM3" s="136"/>
+      <c r="AN3" s="136"/>
+      <c r="AO3" s="136"/>
+      <c r="AP3" s="136"/>
+      <c r="AQ3" s="136"/>
+      <c r="AR3" s="136"/>
+      <c r="AS3" s="136"/>
+      <c r="AT3" s="136"/>
+      <c r="AU3" s="136"/>
+      <c r="AV3" s="136"/>
+      <c r="AW3" s="136"/>
+      <c r="AX3" s="136"/>
+      <c r="AY3" s="136"/>
+      <c r="AZ3" s="136"/>
+      <c r="BA3" s="136"/>
+      <c r="BB3" s="136"/>
+      <c r="BC3" s="136"/>
+      <c r="BD3" s="136"/>
+      <c r="BE3" s="136"/>
+      <c r="BF3" s="136"/>
+      <c r="BG3" s="136"/>
+      <c r="BH3" s="136"/>
+      <c r="BI3" s="136"/>
+      <c r="BJ3" s="136"/>
+      <c r="BK3" s="136"/>
+      <c r="BL3" s="136"/>
+      <c r="BM3" s="136"/>
+      <c r="BN3" s="136"/>
+      <c r="BO3" s="136"/>
+      <c r="BP3" s="136"/>
+      <c r="BQ3" s="146" t="s">
+        <v>75</v>
+      </c>
+      <c r="BR3" s="146"/>
+      <c r="BS3" s="146"/>
+      <c r="BT3" s="146"/>
+      <c r="BU3" s="146"/>
+      <c r="BV3" s="146"/>
+      <c r="BW3" s="146"/>
+      <c r="BX3" s="146"/>
+      <c r="BY3" s="146"/>
+      <c r="BZ3" s="146"/>
+      <c r="CA3" s="146"/>
+      <c r="CB3" s="146"/>
+      <c r="CC3" s="146"/>
+      <c r="CD3" s="146"/>
+      <c r="CE3" s="146"/>
+      <c r="CF3" s="146"/>
+      <c r="CG3" s="146"/>
+      <c r="CH3" s="146"/>
+      <c r="CI3" s="136" t="s">
+        <v>82</v>
+      </c>
+      <c r="CJ3" s="136"/>
+      <c r="CK3" s="136"/>
+      <c r="CL3" s="136"/>
+      <c r="CM3" s="136"/>
+      <c r="CN3" s="136"/>
+      <c r="CO3" s="136"/>
+      <c r="CP3" s="136"/>
+      <c r="CQ3" s="136"/>
+      <c r="CR3" s="136"/>
+      <c r="CS3" s="136"/>
+      <c r="CT3" s="136"/>
       <c r="CU3" s="60"/>
       <c r="CV3" s="60"/>
       <c r="CW3" s="60"/>
@@ -1940,7 +1960,7 @@
       <c r="DN3" s="60"/>
       <c r="DO3" s="60"/>
     </row>
-    <row r="4" spans="1:119" s="17" customFormat="1">
+    <row r="4" spans="1:119" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="109"/>
       <c r="B4" s="61"/>
       <c r="C4" s="21"/>
@@ -2039,9 +2059,9 @@
       <c r="DG4" s="23"/>
       <c r="DH4" s="23"/>
     </row>
-    <row r="5" spans="1:119" s="17" customFormat="1" ht="13">
+    <row r="5" spans="1:119" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A5" s="109" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B5" s="61"/>
       <c r="C5" s="21"/>
@@ -2086,12 +2106,12 @@
       <c r="AT5" s="23"/>
       <c r="AU5" s="23"/>
       <c r="AV5" s="23"/>
-      <c r="AW5" s="145" t="s">
+      <c r="AW5" s="154" t="s">
         <v>48</v>
       </c>
-      <c r="AX5" s="145"/>
-      <c r="AY5" s="145"/>
-      <c r="AZ5" s="145"/>
+      <c r="AX5" s="154"/>
+      <c r="AY5" s="154"/>
+      <c r="AZ5" s="154"/>
       <c r="BA5" s="23"/>
       <c r="BB5" s="23"/>
       <c r="BD5" s="23"/>
@@ -2139,9 +2159,9 @@
       <c r="DG5" s="23"/>
       <c r="DH5" s="23"/>
     </row>
-    <row r="6" spans="1:119" s="17" customFormat="1" ht="13">
+    <row r="6" spans="1:119" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A6" s="109" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B6" s="61"/>
       <c r="C6" s="21"/>
@@ -2161,14 +2181,14 @@
       <c r="Q6" s="22"/>
       <c r="T6" s="62"/>
       <c r="V6" s="23"/>
-      <c r="AA6" s="162" t="s">
-        <v>82</v>
-      </c>
-      <c r="AB6" s="163"/>
-      <c r="AC6" s="163"/>
-      <c r="AD6" s="163"/>
-      <c r="AE6" s="163"/>
-      <c r="AF6" s="163"/>
+      <c r="AA6" s="134" t="s">
+        <v>81</v>
+      </c>
+      <c r="AB6" s="135"/>
+      <c r="AC6" s="135"/>
+      <c r="AD6" s="135"/>
+      <c r="AE6" s="135"/>
+      <c r="AF6" s="135"/>
       <c r="AH6" s="23"/>
       <c r="AI6" s="62"/>
       <c r="AJ6" s="62"/>
@@ -2181,16 +2201,16 @@
       <c r="AT6" s="23"/>
       <c r="AU6" s="62"/>
       <c r="AV6" s="62"/>
-      <c r="AW6" s="160" t="s">
-        <v>81</v>
-      </c>
-      <c r="AX6" s="161"/>
-      <c r="AY6" s="161"/>
-      <c r="AZ6" s="161"/>
-      <c r="BA6" s="161"/>
-      <c r="BB6" s="161"/>
-      <c r="BC6" s="161"/>
-      <c r="BD6" s="161"/>
+      <c r="AW6" s="132" t="s">
+        <v>80</v>
+      </c>
+      <c r="AX6" s="133"/>
+      <c r="AY6" s="133"/>
+      <c r="AZ6" s="133"/>
+      <c r="BA6" s="133"/>
+      <c r="BB6" s="133"/>
+      <c r="BC6" s="133"/>
+      <c r="BD6" s="133"/>
       <c r="BF6" s="23"/>
       <c r="BG6" s="23"/>
       <c r="BH6" s="23"/>
@@ -2214,7 +2234,7 @@
       <c r="CB6" s="23"/>
       <c r="CD6" s="23"/>
       <c r="CE6" s="116" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="CF6" s="110"/>
       <c r="CG6" s="110"/>
@@ -2225,27 +2245,27 @@
       <c r="CL6" s="23"/>
       <c r="CP6" s="23"/>
       <c r="CQ6" s="23"/>
-      <c r="CR6" s="128" t="s">
-        <v>86</v>
-      </c>
-      <c r="CS6" s="129"/>
-      <c r="CT6" s="129"/>
-      <c r="CU6" s="129"/>
-      <c r="CV6" s="129"/>
-      <c r="CW6" s="129"/>
-      <c r="CX6" s="129"/>
-      <c r="CY6" s="129"/>
-      <c r="CZ6" s="129"/>
-      <c r="DA6" s="129"/>
-      <c r="DB6" s="129"/>
-      <c r="DC6" s="129"/>
-      <c r="DD6" s="129"/>
-      <c r="DE6" s="129"/>
+      <c r="CR6" s="158" t="s">
+        <v>85</v>
+      </c>
+      <c r="CS6" s="159"/>
+      <c r="CT6" s="159"/>
+      <c r="CU6" s="159"/>
+      <c r="CV6" s="159"/>
+      <c r="CW6" s="159"/>
+      <c r="CX6" s="159"/>
+      <c r="CY6" s="159"/>
+      <c r="CZ6" s="159"/>
+      <c r="DA6" s="159"/>
+      <c r="DB6" s="159"/>
+      <c r="DC6" s="159"/>
+      <c r="DD6" s="159"/>
+      <c r="DE6" s="159"/>
       <c r="DF6" s="23"/>
       <c r="DG6" s="23"/>
       <c r="DH6" s="23"/>
     </row>
-    <row r="7" spans="1:119" s="17" customFormat="1" ht="13" thickBot="1">
+    <row r="7" spans="1:119" s="17" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="61"/>
       <c r="C7" s="21"/>
       <c r="D7" s="21"/>
@@ -2337,135 +2357,135 @@
       <c r="DG7" s="23"/>
       <c r="DH7" s="23"/>
     </row>
-    <row r="8" spans="1:119">
-      <c r="C8" s="157" t="s">
+    <row r="8" spans="1:119" x14ac:dyDescent="0.2">
+      <c r="C8" s="129" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="158"/>
-      <c r="E8" s="158"/>
-      <c r="F8" s="158"/>
-      <c r="G8" s="158"/>
-      <c r="H8" s="159"/>
-      <c r="I8" s="157" t="s">
+      <c r="D8" s="130"/>
+      <c r="E8" s="130"/>
+      <c r="F8" s="130"/>
+      <c r="G8" s="130"/>
+      <c r="H8" s="131"/>
+      <c r="I8" s="129" t="s">
         <v>14</v>
       </c>
-      <c r="J8" s="158"/>
-      <c r="K8" s="158"/>
-      <c r="L8" s="158"/>
-      <c r="M8" s="158"/>
-      <c r="N8" s="159"/>
-      <c r="O8" s="157" t="s">
+      <c r="J8" s="130"/>
+      <c r="K8" s="130"/>
+      <c r="L8" s="130"/>
+      <c r="M8" s="130"/>
+      <c r="N8" s="131"/>
+      <c r="O8" s="129" t="s">
         <v>15</v>
       </c>
-      <c r="P8" s="158"/>
-      <c r="Q8" s="158"/>
-      <c r="R8" s="158"/>
-      <c r="S8" s="158"/>
-      <c r="T8" s="159"/>
-      <c r="U8" s="157" t="s">
+      <c r="P8" s="130"/>
+      <c r="Q8" s="130"/>
+      <c r="R8" s="130"/>
+      <c r="S8" s="130"/>
+      <c r="T8" s="131"/>
+      <c r="U8" s="129" t="s">
         <v>16</v>
       </c>
-      <c r="V8" s="158"/>
-      <c r="W8" s="158"/>
-      <c r="X8" s="158"/>
-      <c r="Y8" s="158"/>
-      <c r="Z8" s="159"/>
-      <c r="AA8" s="157" t="s">
+      <c r="V8" s="130"/>
+      <c r="W8" s="130"/>
+      <c r="X8" s="130"/>
+      <c r="Y8" s="130"/>
+      <c r="Z8" s="131"/>
+      <c r="AA8" s="129" t="s">
         <v>17</v>
       </c>
-      <c r="AB8" s="158"/>
-      <c r="AC8" s="158"/>
-      <c r="AD8" s="158"/>
-      <c r="AE8" s="158"/>
-      <c r="AF8" s="159"/>
-      <c r="AG8" s="157" t="s">
+      <c r="AB8" s="130"/>
+      <c r="AC8" s="130"/>
+      <c r="AD8" s="130"/>
+      <c r="AE8" s="130"/>
+      <c r="AF8" s="131"/>
+      <c r="AG8" s="129" t="s">
         <v>18</v>
       </c>
-      <c r="AH8" s="158"/>
-      <c r="AI8" s="158"/>
-      <c r="AJ8" s="158"/>
-      <c r="AK8" s="158"/>
-      <c r="AL8" s="159"/>
-      <c r="AM8" s="157" t="s">
+      <c r="AH8" s="130"/>
+      <c r="AI8" s="130"/>
+      <c r="AJ8" s="130"/>
+      <c r="AK8" s="130"/>
+      <c r="AL8" s="131"/>
+      <c r="AM8" s="129" t="s">
         <v>19</v>
       </c>
-      <c r="AN8" s="158"/>
-      <c r="AO8" s="158"/>
-      <c r="AP8" s="158"/>
-      <c r="AQ8" s="158"/>
-      <c r="AR8" s="159"/>
-      <c r="AS8" s="157" t="s">
+      <c r="AN8" s="130"/>
+      <c r="AO8" s="130"/>
+      <c r="AP8" s="130"/>
+      <c r="AQ8" s="130"/>
+      <c r="AR8" s="131"/>
+      <c r="AS8" s="129" t="s">
         <v>20</v>
       </c>
-      <c r="AT8" s="158"/>
-      <c r="AU8" s="158"/>
-      <c r="AV8" s="158"/>
-      <c r="AW8" s="158"/>
-      <c r="AX8" s="159"/>
-      <c r="AY8" s="157" t="s">
+      <c r="AT8" s="130"/>
+      <c r="AU8" s="130"/>
+      <c r="AV8" s="130"/>
+      <c r="AW8" s="130"/>
+      <c r="AX8" s="131"/>
+      <c r="AY8" s="129" t="s">
         <v>21</v>
       </c>
-      <c r="AZ8" s="158"/>
-      <c r="BA8" s="158"/>
-      <c r="BB8" s="158"/>
-      <c r="BC8" s="158"/>
-      <c r="BD8" s="159"/>
-      <c r="BE8" s="157" t="s">
+      <c r="AZ8" s="130"/>
+      <c r="BA8" s="130"/>
+      <c r="BB8" s="130"/>
+      <c r="BC8" s="130"/>
+      <c r="BD8" s="131"/>
+      <c r="BE8" s="129" t="s">
         <v>22</v>
       </c>
-      <c r="BF8" s="158"/>
-      <c r="BG8" s="158"/>
-      <c r="BH8" s="158"/>
-      <c r="BI8" s="158"/>
-      <c r="BJ8" s="159"/>
-      <c r="BK8" s="157" t="s">
+      <c r="BF8" s="130"/>
+      <c r="BG8" s="130"/>
+      <c r="BH8" s="130"/>
+      <c r="BI8" s="130"/>
+      <c r="BJ8" s="131"/>
+      <c r="BK8" s="129" t="s">
         <v>23</v>
       </c>
-      <c r="BL8" s="158"/>
-      <c r="BM8" s="158"/>
-      <c r="BN8" s="158"/>
-      <c r="BO8" s="158"/>
-      <c r="BP8" s="159"/>
-      <c r="BQ8" s="157" t="s">
+      <c r="BL8" s="130"/>
+      <c r="BM8" s="130"/>
+      <c r="BN8" s="130"/>
+      <c r="BO8" s="130"/>
+      <c r="BP8" s="131"/>
+      <c r="BQ8" s="129" t="s">
         <v>24</v>
       </c>
-      <c r="BR8" s="158"/>
-      <c r="BS8" s="158"/>
-      <c r="BT8" s="158"/>
-      <c r="BU8" s="158"/>
-      <c r="BV8" s="159"/>
-      <c r="BW8" s="157" t="s">
+      <c r="BR8" s="130"/>
+      <c r="BS8" s="130"/>
+      <c r="BT8" s="130"/>
+      <c r="BU8" s="130"/>
+      <c r="BV8" s="131"/>
+      <c r="BW8" s="129" t="s">
         <v>25</v>
       </c>
-      <c r="BX8" s="158"/>
-      <c r="BY8" s="158"/>
-      <c r="BZ8" s="158"/>
-      <c r="CA8" s="158"/>
-      <c r="CB8" s="159"/>
-      <c r="CC8" s="157" t="s">
+      <c r="BX8" s="130"/>
+      <c r="BY8" s="130"/>
+      <c r="BZ8" s="130"/>
+      <c r="CA8" s="130"/>
+      <c r="CB8" s="131"/>
+      <c r="CC8" s="129" t="s">
         <v>5</v>
       </c>
-      <c r="CD8" s="158"/>
-      <c r="CE8" s="158"/>
-      <c r="CF8" s="158"/>
-      <c r="CG8" s="158"/>
-      <c r="CH8" s="159"/>
-      <c r="CI8" s="157" t="s">
+      <c r="CD8" s="130"/>
+      <c r="CE8" s="130"/>
+      <c r="CF8" s="130"/>
+      <c r="CG8" s="130"/>
+      <c r="CH8" s="131"/>
+      <c r="CI8" s="129" t="s">
         <v>6</v>
       </c>
-      <c r="CJ8" s="158"/>
-      <c r="CK8" s="158"/>
-      <c r="CL8" s="158"/>
-      <c r="CM8" s="158"/>
-      <c r="CN8" s="159"/>
-      <c r="CO8" s="157" t="s">
+      <c r="CJ8" s="130"/>
+      <c r="CK8" s="130"/>
+      <c r="CL8" s="130"/>
+      <c r="CM8" s="130"/>
+      <c r="CN8" s="131"/>
+      <c r="CO8" s="129" t="s">
         <v>7</v>
       </c>
-      <c r="CP8" s="158"/>
-      <c r="CQ8" s="158"/>
-      <c r="CR8" s="158"/>
-      <c r="CS8" s="158"/>
-      <c r="CT8" s="159"/>
+      <c r="CP8" s="130"/>
+      <c r="CQ8" s="130"/>
+      <c r="CR8" s="130"/>
+      <c r="CS8" s="130"/>
+      <c r="CT8" s="131"/>
       <c r="CV8" s="80"/>
       <c r="CW8" s="80"/>
       <c r="CX8" s="80"/>
@@ -2480,200 +2500,200 @@
       <c r="DG8" s="80"/>
       <c r="DH8" s="80"/>
     </row>
-    <row r="9" spans="1:119" s="16" customFormat="1">
+    <row r="9" spans="1:119" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="15" t="s">
         <v>27</v>
       </c>
       <c r="B9" s="15"/>
-      <c r="C9" s="153" t="s">
+      <c r="C9" s="140" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="154"/>
+      <c r="D9" s="141"/>
       <c r="E9" s="69"/>
       <c r="F9" s="69"/>
-      <c r="G9" s="155" t="s">
+      <c r="G9" s="142" t="s">
         <v>28</v>
       </c>
-      <c r="H9" s="156"/>
-      <c r="I9" s="150">
+      <c r="H9" s="143"/>
+      <c r="I9" s="144">
         <v>40959</v>
       </c>
-      <c r="J9" s="154"/>
+      <c r="J9" s="141"/>
       <c r="K9" s="69"/>
       <c r="L9" s="69"/>
-      <c r="M9" s="151">
+      <c r="M9" s="138">
         <f>SUM(I9+6)</f>
         <v>40965</v>
       </c>
-      <c r="N9" s="152"/>
-      <c r="O9" s="150">
+      <c r="N9" s="139"/>
+      <c r="O9" s="144">
         <f>SUM(M9+1)</f>
         <v>40966</v>
       </c>
-      <c r="P9" s="151"/>
+      <c r="P9" s="138"/>
       <c r="Q9" s="70"/>
       <c r="R9" s="70"/>
-      <c r="S9" s="151">
+      <c r="S9" s="138">
         <f>SUM(O9+6)</f>
         <v>40972</v>
       </c>
-      <c r="T9" s="152"/>
-      <c r="U9" s="150">
+      <c r="T9" s="139"/>
+      <c r="U9" s="144">
         <f>SUM(S9+1)</f>
         <v>40973</v>
       </c>
-      <c r="V9" s="151"/>
+      <c r="V9" s="138"/>
       <c r="W9" s="70"/>
       <c r="X9" s="70"/>
-      <c r="Y9" s="151">
+      <c r="Y9" s="138">
         <f>SUM(U9+6)</f>
         <v>40979</v>
       </c>
-      <c r="Z9" s="152"/>
-      <c r="AA9" s="150">
+      <c r="Z9" s="139"/>
+      <c r="AA9" s="144">
         <f>SUM(Y9+1)</f>
         <v>40980</v>
       </c>
-      <c r="AB9" s="151"/>
+      <c r="AB9" s="138"/>
       <c r="AC9" s="70"/>
       <c r="AD9" s="70"/>
-      <c r="AE9" s="151">
+      <c r="AE9" s="138">
         <f>SUM(AA9+6)</f>
         <v>40986</v>
       </c>
-      <c r="AF9" s="152"/>
-      <c r="AG9" s="150">
+      <c r="AF9" s="139"/>
+      <c r="AG9" s="144">
         <f>SUM(AE9+1)</f>
         <v>40987</v>
       </c>
-      <c r="AH9" s="151"/>
+      <c r="AH9" s="138"/>
       <c r="AI9" s="70"/>
       <c r="AJ9" s="70"/>
-      <c r="AK9" s="151">
+      <c r="AK9" s="138">
         <f>SUM(AG9+6)</f>
         <v>40993</v>
       </c>
-      <c r="AL9" s="152"/>
-      <c r="AM9" s="150">
+      <c r="AL9" s="139"/>
+      <c r="AM9" s="144">
         <f>SUM(AK9+1)</f>
         <v>40994</v>
       </c>
-      <c r="AN9" s="151"/>
+      <c r="AN9" s="138"/>
       <c r="AO9" s="70"/>
       <c r="AP9" s="70"/>
-      <c r="AQ9" s="151">
+      <c r="AQ9" s="138">
         <f>SUM(AM9+6)</f>
         <v>41000</v>
       </c>
-      <c r="AR9" s="152"/>
-      <c r="AS9" s="150">
+      <c r="AR9" s="139"/>
+      <c r="AS9" s="144">
         <f>SUM(AQ9+1)</f>
         <v>41001</v>
       </c>
-      <c r="AT9" s="151"/>
+      <c r="AT9" s="138"/>
       <c r="AU9" s="70"/>
       <c r="AV9" s="70"/>
-      <c r="AW9" s="151">
+      <c r="AW9" s="138">
         <f>SUM(AS9+6)</f>
         <v>41007</v>
       </c>
-      <c r="AX9" s="152"/>
-      <c r="AY9" s="150">
+      <c r="AX9" s="139"/>
+      <c r="AY9" s="144">
         <f>SUM(AW9+1)</f>
         <v>41008</v>
       </c>
-      <c r="AZ9" s="151"/>
+      <c r="AZ9" s="138"/>
       <c r="BA9" s="70"/>
       <c r="BB9" s="70"/>
-      <c r="BC9" s="151">
+      <c r="BC9" s="138">
         <f>SUM(AY9+6)</f>
         <v>41014</v>
       </c>
-      <c r="BD9" s="152"/>
-      <c r="BE9" s="150">
+      <c r="BD9" s="139"/>
+      <c r="BE9" s="144">
         <f>SUM(BC9+1)</f>
         <v>41015</v>
       </c>
-      <c r="BF9" s="151"/>
+      <c r="BF9" s="138"/>
       <c r="BG9" s="70"/>
       <c r="BH9" s="70"/>
-      <c r="BI9" s="151">
+      <c r="BI9" s="138">
         <f>SUM(BE9+6)</f>
         <v>41021</v>
       </c>
-      <c r="BJ9" s="152"/>
-      <c r="BK9" s="150">
+      <c r="BJ9" s="139"/>
+      <c r="BK9" s="144">
         <f>SUM(BI9+1)</f>
         <v>41022</v>
       </c>
-      <c r="BL9" s="151"/>
+      <c r="BL9" s="138"/>
       <c r="BM9" s="70"/>
       <c r="BN9" s="70"/>
-      <c r="BO9" s="151">
+      <c r="BO9" s="138">
         <f>SUM(BK9+6)</f>
         <v>41028</v>
       </c>
-      <c r="BP9" s="152"/>
-      <c r="BQ9" s="150">
+      <c r="BP9" s="139"/>
+      <c r="BQ9" s="144">
         <f>SUM(BO9+1)</f>
         <v>41029</v>
       </c>
-      <c r="BR9" s="151"/>
+      <c r="BR9" s="138"/>
       <c r="BS9" s="70"/>
       <c r="BT9" s="70"/>
-      <c r="BU9" s="151">
+      <c r="BU9" s="138">
         <f>SUM(BQ9+6)</f>
         <v>41035</v>
       </c>
-      <c r="BV9" s="152"/>
-      <c r="BW9" s="150">
+      <c r="BV9" s="139"/>
+      <c r="BW9" s="144">
         <f>SUM(BU9+1)</f>
         <v>41036</v>
       </c>
-      <c r="BX9" s="151"/>
+      <c r="BX9" s="138"/>
       <c r="BY9" s="70"/>
       <c r="BZ9" s="70"/>
-      <c r="CA9" s="151">
+      <c r="CA9" s="138">
         <f>SUM(BW9+6)</f>
         <v>41042</v>
       </c>
-      <c r="CB9" s="152"/>
-      <c r="CC9" s="150">
+      <c r="CB9" s="139"/>
+      <c r="CC9" s="144">
         <f>SUM(CA9+1)</f>
         <v>41043</v>
       </c>
-      <c r="CD9" s="151"/>
+      <c r="CD9" s="138"/>
       <c r="CE9" s="70"/>
       <c r="CF9" s="70"/>
-      <c r="CG9" s="151">
+      <c r="CG9" s="138">
         <f>SUM(CC9+6)</f>
         <v>41049</v>
       </c>
-      <c r="CH9" s="152"/>
-      <c r="CI9" s="150">
+      <c r="CH9" s="139"/>
+      <c r="CI9" s="144">
         <f>SUM(CG9+1)</f>
         <v>41050</v>
       </c>
-      <c r="CJ9" s="151"/>
+      <c r="CJ9" s="138"/>
       <c r="CK9" s="70"/>
       <c r="CL9" s="70"/>
-      <c r="CM9" s="151">
+      <c r="CM9" s="138">
         <f>SUM(CI9+6)</f>
         <v>41056</v>
       </c>
-      <c r="CN9" s="152"/>
-      <c r="CO9" s="150">
+      <c r="CN9" s="139"/>
+      <c r="CO9" s="144">
         <f>SUM(CM9+1)</f>
         <v>41057</v>
       </c>
-      <c r="CP9" s="151"/>
+      <c r="CP9" s="138"/>
       <c r="CQ9" s="70"/>
       <c r="CR9" s="70"/>
-      <c r="CS9" s="151">
+      <c r="CS9" s="138">
         <f>SUM(CO9+6)</f>
         <v>41063</v>
       </c>
-      <c r="CT9" s="152"/>
+      <c r="CT9" s="139"/>
       <c r="CV9" s="62"/>
       <c r="CW9" s="62"/>
       <c r="CX9" s="68"/>
@@ -2688,7 +2708,7 @@
       <c r="DG9" s="62"/>
       <c r="DH9" s="62"/>
     </row>
-    <row r="10" spans="1:119" s="8" customFormat="1">
+    <row r="10" spans="1:119" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="77"/>
@@ -2801,7 +2821,7 @@
       <c r="DG10" s="80"/>
       <c r="DH10" s="80"/>
     </row>
-    <row r="11" spans="1:119" s="8" customFormat="1">
+    <row r="11" spans="1:119" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="73"/>
@@ -2914,7 +2934,7 @@
       <c r="DG11" s="81"/>
       <c r="DH11" s="81"/>
     </row>
-    <row r="12" spans="1:119" s="8" customFormat="1">
+    <row r="12" spans="1:119" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>0</v>
       </c>
@@ -3029,9 +3049,9 @@
       <c r="DG12" s="81"/>
       <c r="DH12" s="82"/>
     </row>
-    <row r="13" spans="1:119">
+    <row r="13" spans="1:119" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B13" s="47"/>
       <c r="C13" s="83"/>
@@ -3144,9 +3164,9 @@
       <c r="DG13" s="85"/>
       <c r="DH13" s="84"/>
     </row>
-    <row r="14" spans="1:119">
+    <row r="14" spans="1:119" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B14" s="48"/>
       <c r="C14" s="24"/>
@@ -3260,25 +3280,25 @@
       <c r="DG14" s="88"/>
       <c r="DH14" s="87"/>
     </row>
-    <row r="15" spans="1:119">
+    <row r="15" spans="1:119" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B15" s="48"/>
       <c r="C15" s="24"/>
       <c r="D15" s="25"/>
       <c r="E15" s="25"/>
       <c r="F15" s="25"/>
-      <c r="G15" s="133"/>
-      <c r="H15" s="133"/>
-      <c r="I15" s="133"/>
-      <c r="J15" s="133"/>
-      <c r="K15" s="133"/>
-      <c r="L15" s="133"/>
-      <c r="M15" s="133"/>
-      <c r="N15" s="133"/>
-      <c r="O15" s="133"/>
-      <c r="P15" s="133"/>
+      <c r="G15" s="128"/>
+      <c r="H15" s="128"/>
+      <c r="I15" s="128"/>
+      <c r="J15" s="128"/>
+      <c r="K15" s="128"/>
+      <c r="L15" s="128"/>
+      <c r="M15" s="128"/>
+      <c r="N15" s="128"/>
+      <c r="O15" s="128"/>
+      <c r="P15" s="128"/>
       <c r="Q15" s="25"/>
       <c r="R15" s="25"/>
       <c r="S15" s="26"/>
@@ -3376,7 +3396,7 @@
       <c r="DG15" s="88"/>
       <c r="DH15" s="87"/>
     </row>
-    <row r="16" spans="1:119">
+    <row r="16" spans="1:119" x14ac:dyDescent="0.2">
       <c r="A16" s="9"/>
       <c r="B16" s="48"/>
       <c r="C16" s="24"/>
@@ -3490,7 +3510,7 @@
       <c r="DG16" s="88"/>
       <c r="DH16" s="87"/>
     </row>
-    <row r="17" spans="1:112">
+    <row r="17" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>8</v>
       </c>
@@ -3605,9 +3625,9 @@
       <c r="DG17" s="85"/>
       <c r="DH17" s="84"/>
     </row>
-    <row r="18" spans="1:112">
+    <row r="18" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B18" s="48"/>
       <c r="C18" s="24"/>
@@ -3624,15 +3644,15 @@
       <c r="N18" s="27"/>
       <c r="O18" s="24"/>
       <c r="P18" s="25"/>
-      <c r="Q18" s="147"/>
-      <c r="R18" s="147"/>
-      <c r="S18" s="147"/>
-      <c r="T18" s="147"/>
-      <c r="U18" s="147"/>
-      <c r="V18" s="147"/>
-      <c r="W18" s="147"/>
-      <c r="X18" s="147"/>
-      <c r="Y18" s="147"/>
+      <c r="Q18" s="156"/>
+      <c r="R18" s="156"/>
+      <c r="S18" s="156"/>
+      <c r="T18" s="156"/>
+      <c r="U18" s="156"/>
+      <c r="V18" s="156"/>
+      <c r="W18" s="156"/>
+      <c r="X18" s="156"/>
+      <c r="Y18" s="156"/>
       <c r="Z18" s="27"/>
       <c r="AA18" s="24"/>
       <c r="AB18" s="25"/>
@@ -3721,7 +3741,7 @@
       <c r="DG18" s="88"/>
       <c r="DH18" s="87"/>
     </row>
-    <row r="19" spans="1:112">
+    <row r="19" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="s">
         <v>43</v>
       </c>
@@ -3837,9 +3857,9 @@
       <c r="DG19" s="88"/>
       <c r="DH19" s="87"/>
     </row>
-    <row r="20" spans="1:112">
+    <row r="20" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A20" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B20" s="48"/>
       <c r="C20" s="24"/>
@@ -3866,9 +3886,9 @@
       <c r="X20" s="25"/>
       <c r="Y20" s="26"/>
       <c r="Z20" s="27"/>
-      <c r="AA20" s="148"/>
-      <c r="AB20" s="147"/>
-      <c r="AC20" s="147"/>
+      <c r="AA20" s="157"/>
+      <c r="AB20" s="156"/>
+      <c r="AC20" s="156"/>
       <c r="AD20" s="25"/>
       <c r="AE20" s="26"/>
       <c r="AF20" s="27"/>
@@ -3953,7 +3973,7 @@
       <c r="DG20" s="88"/>
       <c r="DH20" s="87"/>
     </row>
-    <row r="21" spans="1:112">
+    <row r="21" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A21" s="4"/>
       <c r="B21" s="66"/>
       <c r="C21" s="24"/>
@@ -4067,7 +4087,7 @@
       <c r="DG21" s="88"/>
       <c r="DH21" s="87"/>
     </row>
-    <row r="22" spans="1:112">
+    <row r="22" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>2</v>
       </c>
@@ -4182,9 +4202,9 @@
       <c r="DG22" s="85"/>
       <c r="DH22" s="84"/>
     </row>
-    <row r="23" spans="1:112">
+    <row r="23" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A23" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B23" s="48"/>
       <c r="C23" s="24"/>
@@ -4209,18 +4229,18 @@
       <c r="V23" s="25"/>
       <c r="W23" s="25"/>
       <c r="X23" s="25"/>
-      <c r="Y23" s="141"/>
-      <c r="Z23" s="141"/>
-      <c r="AA23" s="141"/>
-      <c r="AB23" s="141"/>
-      <c r="AC23" s="141"/>
-      <c r="AD23" s="141"/>
-      <c r="AE23" s="141"/>
-      <c r="AF23" s="141"/>
-      <c r="AG23" s="141"/>
-      <c r="AH23" s="141"/>
-      <c r="AI23" s="143"/>
-      <c r="AJ23" s="143"/>
+      <c r="Y23" s="150"/>
+      <c r="Z23" s="150"/>
+      <c r="AA23" s="150"/>
+      <c r="AB23" s="150"/>
+      <c r="AC23" s="150"/>
+      <c r="AD23" s="150"/>
+      <c r="AE23" s="150"/>
+      <c r="AF23" s="150"/>
+      <c r="AG23" s="150"/>
+      <c r="AH23" s="150"/>
+      <c r="AI23" s="152"/>
+      <c r="AJ23" s="152"/>
       <c r="AK23" s="26"/>
       <c r="AL23" s="27"/>
       <c r="AM23" s="24"/>
@@ -4298,9 +4318,9 @@
       <c r="DG23" s="88"/>
       <c r="DH23" s="87"/>
     </row>
-    <row r="24" spans="1:112">
+    <row r="24" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A24" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B24" s="48"/>
       <c r="C24" s="24"/>
@@ -4339,12 +4359,12 @@
       <c r="AJ24" s="25"/>
       <c r="AK24" s="26"/>
       <c r="AL24" s="27"/>
-      <c r="AS24" s="140"/>
-      <c r="AT24" s="141"/>
-      <c r="AU24" s="141"/>
-      <c r="AV24" s="141"/>
-      <c r="AW24" s="141"/>
-      <c r="AX24" s="142"/>
+      <c r="AS24" s="149"/>
+      <c r="AT24" s="150"/>
+      <c r="AU24" s="150"/>
+      <c r="AV24" s="150"/>
+      <c r="AW24" s="150"/>
+      <c r="AX24" s="151"/>
       <c r="AY24" s="24"/>
       <c r="AZ24" s="25"/>
       <c r="BA24" s="26"/>
@@ -4408,9 +4428,9 @@
       <c r="DG24" s="88"/>
       <c r="DH24" s="87"/>
     </row>
-    <row r="25" spans="1:112">
+    <row r="25" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A25" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B25" s="48"/>
       <c r="C25" s="24"/>
@@ -4437,14 +4457,14 @@
       <c r="X25" s="25"/>
       <c r="Y25" s="26"/>
       <c r="Z25" s="27"/>
-      <c r="AA25" s="140"/>
-      <c r="AB25" s="141"/>
-      <c r="AC25" s="141"/>
-      <c r="AD25" s="141"/>
-      <c r="AE25" s="141"/>
-      <c r="AF25" s="141"/>
-      <c r="AG25" s="141"/>
-      <c r="AH25" s="141"/>
+      <c r="AA25" s="149"/>
+      <c r="AB25" s="150"/>
+      <c r="AC25" s="150"/>
+      <c r="AD25" s="150"/>
+      <c r="AE25" s="150"/>
+      <c r="AF25" s="150"/>
+      <c r="AG25" s="150"/>
+      <c r="AH25" s="150"/>
       <c r="AI25" s="26"/>
       <c r="AJ25" s="25"/>
       <c r="AK25" s="26"/>
@@ -4524,9 +4544,9 @@
       <c r="DG25" s="88"/>
       <c r="DH25" s="87"/>
     </row>
-    <row r="26" spans="1:112">
+    <row r="26" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A26" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B26" s="48"/>
       <c r="C26" s="24"/>
@@ -4561,9 +4581,9 @@
       <c r="AF26" s="27"/>
       <c r="AG26" s="24"/>
       <c r="AH26" s="25"/>
-      <c r="AI26" s="141"/>
-      <c r="AJ26" s="141"/>
-      <c r="AK26" s="141"/>
+      <c r="AI26" s="150"/>
+      <c r="AJ26" s="150"/>
+      <c r="AK26" s="150"/>
       <c r="AL26" s="27"/>
       <c r="AM26" s="24"/>
       <c r="AN26" s="25"/>
@@ -4640,9 +4660,9 @@
       <c r="DG26" s="88"/>
       <c r="DH26" s="87"/>
     </row>
-    <row r="27" spans="1:112">
+    <row r="27" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A27" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B27" s="48"/>
       <c r="C27" s="24"/>
@@ -4680,9 +4700,9 @@
       <c r="AI27" s="26"/>
       <c r="AM27" s="113"/>
       <c r="AS27" s="113"/>
-      <c r="AW27" s="144"/>
-      <c r="AX27" s="144"/>
-      <c r="AY27" s="144"/>
+      <c r="AW27" s="153"/>
+      <c r="AX27" s="153"/>
+      <c r="AY27" s="153"/>
       <c r="BA27" s="26"/>
       <c r="BB27" s="25"/>
       <c r="BC27" s="26"/>
@@ -4744,9 +4764,9 @@
       <c r="DG27" s="88"/>
       <c r="DH27" s="87"/>
     </row>
-    <row r="28" spans="1:112">
+    <row r="28" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A28" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B28" s="48"/>
       <c r="C28" s="24"/>
@@ -4781,9 +4801,9 @@
       <c r="AF28" s="27"/>
       <c r="AG28" s="24"/>
       <c r="AH28" s="25"/>
-      <c r="AI28" s="141"/>
-      <c r="AJ28" s="141"/>
-      <c r="AK28" s="141"/>
+      <c r="AI28" s="150"/>
+      <c r="AJ28" s="150"/>
+      <c r="AK28" s="150"/>
       <c r="AL28" s="27"/>
       <c r="AM28" s="24"/>
       <c r="AN28" s="25"/>
@@ -4860,7 +4880,7 @@
       <c r="DG28" s="88"/>
       <c r="DH28" s="87"/>
     </row>
-    <row r="29" spans="1:112">
+    <row r="29" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A29" s="9" t="s">
         <v>44</v>
       </c>
@@ -4976,7 +4996,7 @@
       <c r="DG29" s="88"/>
       <c r="DH29" s="87"/>
     </row>
-    <row r="30" spans="1:112">
+    <row r="30" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A30" s="5"/>
       <c r="B30" s="67"/>
       <c r="C30" s="24"/>
@@ -5090,7 +5110,7 @@
       <c r="DG30" s="88"/>
       <c r="DH30" s="87"/>
     </row>
-    <row r="31" spans="1:112">
+    <row r="31" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>3</v>
       </c>
@@ -5193,9 +5213,9 @@
       <c r="DG31" s="85"/>
       <c r="DH31" s="84"/>
     </row>
-    <row r="32" spans="1:112">
+    <row r="32" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A32" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B32" s="48"/>
       <c r="C32" s="24"/>
@@ -5231,20 +5251,20 @@
       <c r="AG32" s="24"/>
       <c r="AH32" s="25"/>
       <c r="AI32" s="26"/>
-      <c r="AJ32" s="149"/>
-      <c r="AK32" s="149"/>
-      <c r="AL32" s="149"/>
-      <c r="AM32" s="149"/>
-      <c r="AN32" s="149"/>
-      <c r="AO32" s="149"/>
-      <c r="AP32" s="149"/>
-      <c r="AQ32" s="149"/>
-      <c r="AR32" s="149"/>
-      <c r="AS32" s="149"/>
-      <c r="AT32" s="149"/>
-      <c r="AU32" s="149"/>
-      <c r="AV32" s="149"/>
-      <c r="AW32" s="149"/>
+      <c r="AJ32" s="164"/>
+      <c r="AK32" s="164"/>
+      <c r="AL32" s="164"/>
+      <c r="AM32" s="164"/>
+      <c r="AN32" s="164"/>
+      <c r="AO32" s="164"/>
+      <c r="AP32" s="164"/>
+      <c r="AQ32" s="164"/>
+      <c r="AR32" s="164"/>
+      <c r="AS32" s="164"/>
+      <c r="AT32" s="164"/>
+      <c r="AU32" s="164"/>
+      <c r="AV32" s="164"/>
+      <c r="AW32" s="164"/>
       <c r="AX32" s="27"/>
       <c r="AY32" s="24"/>
       <c r="AZ32" s="25"/>
@@ -5309,9 +5329,9 @@
       <c r="DG32" s="88"/>
       <c r="DH32" s="87"/>
     </row>
-    <row r="33" spans="1:112">
+    <row r="33" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A33" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B33" s="48"/>
       <c r="C33" s="24"/>
@@ -5425,9 +5445,9 @@
       <c r="DG33" s="88"/>
       <c r="DH33" s="87"/>
     </row>
-    <row r="34" spans="1:112">
+    <row r="34" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A34" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B34" s="48"/>
       <c r="C34" s="24"/>
@@ -5463,23 +5483,23 @@
       <c r="AG34" s="24"/>
       <c r="AH34" s="25"/>
       <c r="AI34" s="26"/>
-      <c r="AJ34" s="146"/>
-      <c r="AK34" s="146"/>
-      <c r="AL34" s="146"/>
-      <c r="AM34" s="146"/>
-      <c r="AN34" s="146"/>
-      <c r="AO34" s="146"/>
-      <c r="AP34" s="146"/>
-      <c r="AQ34" s="146"/>
-      <c r="AR34" s="146"/>
-      <c r="AS34" s="146"/>
-      <c r="AT34" s="146"/>
-      <c r="AU34" s="146"/>
-      <c r="AV34" s="146"/>
-      <c r="AW34" s="146"/>
-      <c r="AX34" s="146"/>
-      <c r="AY34" s="146"/>
-      <c r="AZ34" s="146"/>
+      <c r="AJ34" s="155"/>
+      <c r="AK34" s="155"/>
+      <c r="AL34" s="155"/>
+      <c r="AM34" s="155"/>
+      <c r="AN34" s="155"/>
+      <c r="AO34" s="155"/>
+      <c r="AP34" s="155"/>
+      <c r="AQ34" s="155"/>
+      <c r="AR34" s="155"/>
+      <c r="AS34" s="155"/>
+      <c r="AT34" s="155"/>
+      <c r="AU34" s="155"/>
+      <c r="AV34" s="155"/>
+      <c r="AW34" s="155"/>
+      <c r="AX34" s="155"/>
+      <c r="AY34" s="155"/>
+      <c r="AZ34" s="155"/>
       <c r="BA34" s="26"/>
       <c r="BB34" s="25"/>
       <c r="BC34" s="26"/>
@@ -5541,7 +5561,7 @@
       <c r="DG34" s="88"/>
       <c r="DH34" s="87"/>
     </row>
-    <row r="35" spans="1:112">
+    <row r="35" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A35" s="5"/>
       <c r="B35" s="67"/>
       <c r="C35" s="24"/>
@@ -5655,7 +5675,7 @@
       <c r="DG35" s="88"/>
       <c r="DH35" s="87"/>
     </row>
-    <row r="36" spans="1:112">
+    <row r="36" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A36" s="11" t="s">
         <v>4</v>
       </c>
@@ -5739,9 +5759,9 @@
       <c r="DG36" s="85"/>
       <c r="DH36" s="84"/>
     </row>
-    <row r="37" spans="1:112">
+    <row r="37" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A37" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B37" s="48"/>
       <c r="C37" s="24"/>
@@ -5777,39 +5797,39 @@
       <c r="AG37" s="24"/>
       <c r="AH37" s="25"/>
       <c r="AI37" s="26"/>
-      <c r="AJ37" s="138"/>
-      <c r="AK37" s="138"/>
-      <c r="AL37" s="138"/>
-      <c r="AM37" s="138"/>
-      <c r="AN37" s="138"/>
-      <c r="AO37" s="138"/>
-      <c r="AP37" s="138"/>
-      <c r="AQ37" s="138"/>
-      <c r="AR37" s="138"/>
-      <c r="AS37" s="138"/>
-      <c r="AT37" s="138"/>
-      <c r="AU37" s="138"/>
-      <c r="AV37" s="138"/>
-      <c r="AW37" s="138"/>
-      <c r="AX37" s="138"/>
-      <c r="AY37" s="138"/>
-      <c r="AZ37" s="138"/>
-      <c r="BA37" s="138"/>
-      <c r="BB37" s="138"/>
-      <c r="BC37" s="138"/>
-      <c r="BD37" s="138"/>
-      <c r="BE37" s="138"/>
-      <c r="BF37" s="138"/>
-      <c r="BG37" s="138"/>
-      <c r="BH37" s="138"/>
-      <c r="BI37" s="138"/>
-      <c r="BJ37" s="138"/>
-      <c r="BK37" s="138"/>
-      <c r="BL37" s="138"/>
-      <c r="BM37" s="138"/>
-      <c r="BN37" s="138"/>
-      <c r="BO37" s="138"/>
-      <c r="BP37" s="139"/>
+      <c r="AJ37" s="147"/>
+      <c r="AK37" s="147"/>
+      <c r="AL37" s="147"/>
+      <c r="AM37" s="147"/>
+      <c r="AN37" s="147"/>
+      <c r="AO37" s="147"/>
+      <c r="AP37" s="147"/>
+      <c r="AQ37" s="147"/>
+      <c r="AR37" s="147"/>
+      <c r="AS37" s="147"/>
+      <c r="AT37" s="147"/>
+      <c r="AU37" s="147"/>
+      <c r="AV37" s="147"/>
+      <c r="AW37" s="147"/>
+      <c r="AX37" s="147"/>
+      <c r="AY37" s="147"/>
+      <c r="AZ37" s="147"/>
+      <c r="BA37" s="147"/>
+      <c r="BB37" s="147"/>
+      <c r="BC37" s="147"/>
+      <c r="BD37" s="147"/>
+      <c r="BE37" s="147"/>
+      <c r="BF37" s="147"/>
+      <c r="BG37" s="147"/>
+      <c r="BH37" s="147"/>
+      <c r="BI37" s="147"/>
+      <c r="BJ37" s="147"/>
+      <c r="BK37" s="147"/>
+      <c r="BL37" s="147"/>
+      <c r="BM37" s="147"/>
+      <c r="BN37" s="147"/>
+      <c r="BO37" s="147"/>
+      <c r="BP37" s="148"/>
       <c r="BQ37" s="83"/>
       <c r="BR37" s="84"/>
       <c r="BS37" s="85"/>
@@ -5855,7 +5875,7 @@
       <c r="DG37" s="88"/>
       <c r="DH37" s="87"/>
     </row>
-    <row r="38" spans="1:112">
+    <row r="38" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A38" s="9" t="s">
         <v>45</v>
       </c>
@@ -5903,12 +5923,12 @@
       <c r="AQ38" s="26"/>
       <c r="AR38" s="27"/>
       <c r="AS38" s="24"/>
-      <c r="AT38" s="131"/>
-      <c r="AU38" s="131"/>
-      <c r="AV38" s="131"/>
-      <c r="AW38" s="131"/>
-      <c r="AX38" s="131"/>
-      <c r="AY38" s="131"/>
+      <c r="AT38" s="161"/>
+      <c r="AU38" s="161"/>
+      <c r="AV38" s="161"/>
+      <c r="AW38" s="161"/>
+      <c r="AX38" s="161"/>
+      <c r="AY38" s="161"/>
       <c r="AZ38" s="25"/>
       <c r="BA38" s="26"/>
       <c r="BB38" s="25"/>
@@ -5920,14 +5940,14 @@
       <c r="BH38" s="120"/>
       <c r="BI38" s="120"/>
       <c r="BJ38" s="120"/>
-      <c r="BK38" s="130"/>
-      <c r="BL38" s="130"/>
-      <c r="BM38" s="130"/>
-      <c r="BN38" s="130"/>
-      <c r="BO38" s="130"/>
-      <c r="BP38" s="130"/>
-      <c r="BQ38" s="130"/>
-      <c r="BR38" s="130"/>
+      <c r="BK38" s="160"/>
+      <c r="BL38" s="160"/>
+      <c r="BM38" s="160"/>
+      <c r="BN38" s="160"/>
+      <c r="BO38" s="160"/>
+      <c r="BP38" s="160"/>
+      <c r="BQ38" s="160"/>
+      <c r="BR38" s="160"/>
       <c r="BS38" s="120"/>
       <c r="BT38" s="120"/>
       <c r="BU38" s="26"/>
@@ -5971,7 +5991,7 @@
       <c r="DG38" s="88"/>
       <c r="DH38" s="87"/>
     </row>
-    <row r="39" spans="1:112">
+    <row r="39" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A39" s="9"/>
       <c r="B39" s="48"/>
       <c r="C39" s="24"/>
@@ -6085,9 +6105,9 @@
       <c r="DG39" s="88"/>
       <c r="DH39" s="87"/>
     </row>
-    <row r="40" spans="1:112">
+    <row r="40" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A40" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B40" s="49"/>
       <c r="C40" s="83"/>
@@ -6200,9 +6220,9 @@
       <c r="DG40" s="85"/>
       <c r="DH40" s="84"/>
     </row>
-    <row r="41" spans="1:112">
+    <row r="41" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A41" s="59" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B41" s="48"/>
       <c r="C41" s="24"/>
@@ -6274,8 +6294,8 @@
       <c r="BQ41" s="24"/>
       <c r="BR41" s="25"/>
       <c r="BS41" s="26"/>
-      <c r="BT41" s="132"/>
-      <c r="BU41" s="132"/>
+      <c r="BT41" s="162"/>
+      <c r="BU41" s="162"/>
       <c r="BV41" s="27"/>
       <c r="BW41" s="24"/>
       <c r="BX41" s="25"/>
@@ -6316,9 +6336,9 @@
       <c r="DG41" s="88"/>
       <c r="DH41" s="87"/>
     </row>
-    <row r="42" spans="1:112">
+    <row r="42" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A42" s="59" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B42" s="48"/>
       <c r="C42" s="24"/>
@@ -6391,20 +6411,20 @@
       <c r="BR42" s="25"/>
       <c r="BS42" s="26"/>
       <c r="BT42" s="25"/>
-      <c r="BU42" s="133"/>
-      <c r="BV42" s="133"/>
-      <c r="BW42" s="133"/>
-      <c r="BX42" s="133"/>
-      <c r="BY42" s="133"/>
-      <c r="BZ42" s="133"/>
-      <c r="CA42" s="133"/>
-      <c r="CB42" s="133"/>
-      <c r="CC42" s="133"/>
-      <c r="CD42" s="133"/>
-      <c r="CE42" s="133"/>
-      <c r="CF42" s="133"/>
-      <c r="CG42" s="133"/>
-      <c r="CH42" s="134"/>
+      <c r="BU42" s="128"/>
+      <c r="BV42" s="128"/>
+      <c r="BW42" s="128"/>
+      <c r="BX42" s="128"/>
+      <c r="BY42" s="128"/>
+      <c r="BZ42" s="128"/>
+      <c r="CA42" s="128"/>
+      <c r="CB42" s="128"/>
+      <c r="CC42" s="128"/>
+      <c r="CD42" s="128"/>
+      <c r="CE42" s="128"/>
+      <c r="CF42" s="128"/>
+      <c r="CG42" s="128"/>
+      <c r="CH42" s="163"/>
       <c r="CI42" s="24"/>
       <c r="CJ42" s="25"/>
       <c r="CK42" s="26"/>
@@ -6432,9 +6452,9 @@
       <c r="DG42" s="88"/>
       <c r="DH42" s="87"/>
     </row>
-    <row r="43" spans="1:112">
+    <row r="43" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A43" s="59" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B43" s="48"/>
       <c r="C43" s="24"/>
@@ -6548,7 +6568,7 @@
       <c r="DG43" s="88"/>
       <c r="DH43" s="87"/>
     </row>
-    <row r="44" spans="1:112">
+    <row r="44" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A44" s="10"/>
       <c r="B44" s="50"/>
       <c r="C44" s="24"/>
@@ -6662,7 +6682,7 @@
       <c r="DG44" s="88"/>
       <c r="DH44" s="87"/>
     </row>
-    <row r="45" spans="1:112">
+    <row r="45" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A45" s="11" t="s">
         <v>12</v>
       </c>
@@ -6777,7 +6797,7 @@
       <c r="DG45" s="85"/>
       <c r="DH45" s="84"/>
     </row>
-    <row r="46" spans="1:112">
+    <row r="46" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A46" s="59" t="s">
         <v>12</v>
       </c>
@@ -6893,7 +6913,7 @@
       <c r="DG46" s="88"/>
       <c r="DH46" s="87"/>
     </row>
-    <row r="47" spans="1:112">
+    <row r="47" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A47" s="10"/>
       <c r="B47" s="50"/>
       <c r="C47" s="24"/>
@@ -7007,7 +7027,7 @@
       <c r="DG47" s="88"/>
       <c r="DH47" s="87"/>
     </row>
-    <row r="48" spans="1:112">
+    <row r="48" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>1</v>
       </c>
@@ -7122,7 +7142,7 @@
       <c r="DG48" s="85"/>
       <c r="DH48" s="84"/>
     </row>
-    <row r="49" spans="1:112">
+    <row r="49" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A49" s="9" t="s">
         <v>31</v>
       </c>
@@ -7238,7 +7258,7 @@
       <c r="DG49" s="88"/>
       <c r="DH49" s="87"/>
     </row>
-    <row r="50" spans="1:112">
+    <row r="50" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A50" s="9" t="s">
         <v>32</v>
       </c>
@@ -7354,7 +7374,7 @@
       <c r="DG50" s="88"/>
       <c r="DH50" s="87"/>
     </row>
-    <row r="51" spans="1:112" ht="13" thickBot="1">
+    <row r="51" spans="1:112" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A51" s="4"/>
       <c r="B51" s="66"/>
       <c r="C51" s="95"/>
@@ -7468,7 +7488,7 @@
       <c r="DG51" s="88"/>
       <c r="DH51" s="87"/>
     </row>
-    <row r="52" spans="1:112">
+    <row r="52" spans="1:112" x14ac:dyDescent="0.2">
       <c r="B52" s="67"/>
       <c r="C52" s="28"/>
       <c r="D52" s="88"/>
@@ -7494,7 +7514,7 @@
       <c r="X52" s="6"/>
       <c r="Y52" s="6"/>
     </row>
-    <row r="53" spans="1:112" s="8" customFormat="1">
+    <row r="53" spans="1:112" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="1"/>
       <c r="B53" s="74"/>
       <c r="D53" s="18"/>
@@ -7509,7 +7529,7 @@
       <c r="M53" s="93"/>
       <c r="N53" s="18"/>
     </row>
-    <row r="54" spans="1:112" s="8" customFormat="1">
+    <row r="54" spans="1:112" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A54" s="1"/>
       <c r="B54" s="74"/>
       <c r="D54" s="94"/>
@@ -7524,7 +7544,7 @@
       <c r="M54" s="94"/>
       <c r="N54" s="94"/>
     </row>
-    <row r="55" spans="1:112" s="8" customFormat="1">
+    <row r="55" spans="1:112" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -7552,7 +7572,7 @@
       <c r="Y55" s="7"/>
       <c r="Z55" s="7"/>
     </row>
-    <row r="56" spans="1:112" s="8" customFormat="1">
+    <row r="56" spans="1:112" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -7582,6 +7602,65 @@
     </row>
   </sheetData>
   <mergeCells count="75">
+    <mergeCell ref="CR6:DE6"/>
+    <mergeCell ref="BK38:BR38"/>
+    <mergeCell ref="AT38:AY38"/>
+    <mergeCell ref="BT41:BU41"/>
+    <mergeCell ref="BU42:CH42"/>
+    <mergeCell ref="AJ32:AW32"/>
+    <mergeCell ref="CO9:CP9"/>
+    <mergeCell ref="CS9:CT9"/>
+    <mergeCell ref="BW9:BX9"/>
+    <mergeCell ref="CA9:CB9"/>
+    <mergeCell ref="CC9:CD9"/>
+    <mergeCell ref="CG9:CH9"/>
+    <mergeCell ref="CI9:CJ9"/>
+    <mergeCell ref="CM9:CN9"/>
+    <mergeCell ref="BU9:BV9"/>
+    <mergeCell ref="AM9:AN9"/>
+    <mergeCell ref="I3:V3"/>
+    <mergeCell ref="W3:AH3"/>
+    <mergeCell ref="AI3:BP3"/>
+    <mergeCell ref="BQ3:CH3"/>
+    <mergeCell ref="AJ37:BP37"/>
+    <mergeCell ref="AS24:AX24"/>
+    <mergeCell ref="AI23:AJ23"/>
+    <mergeCell ref="AI26:AK26"/>
+    <mergeCell ref="AI28:AK28"/>
+    <mergeCell ref="AW27:AY27"/>
+    <mergeCell ref="AW5:AZ5"/>
+    <mergeCell ref="AJ34:AZ34"/>
+    <mergeCell ref="Q18:Y18"/>
+    <mergeCell ref="AA20:AC20"/>
+    <mergeCell ref="Y23:AH23"/>
+    <mergeCell ref="AA25:AH25"/>
+    <mergeCell ref="AQ9:AR9"/>
+    <mergeCell ref="AS9:AT9"/>
+    <mergeCell ref="AW9:AX9"/>
+    <mergeCell ref="AY9:AZ9"/>
+    <mergeCell ref="BC9:BD9"/>
+    <mergeCell ref="BE9:BF9"/>
+    <mergeCell ref="BI9:BJ9"/>
+    <mergeCell ref="BK9:BL9"/>
+    <mergeCell ref="BO9:BP9"/>
+    <mergeCell ref="BQ9:BR9"/>
+    <mergeCell ref="AK9:AL9"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="S9:T9"/>
+    <mergeCell ref="U9:V9"/>
+    <mergeCell ref="Y9:Z9"/>
+    <mergeCell ref="AA9:AB9"/>
+    <mergeCell ref="AE9:AF9"/>
+    <mergeCell ref="AG9:AH9"/>
+    <mergeCell ref="AS8:AX8"/>
+    <mergeCell ref="AY8:BD8"/>
+    <mergeCell ref="BE8:BJ8"/>
+    <mergeCell ref="BK8:BP8"/>
+    <mergeCell ref="BQ8:BV8"/>
     <mergeCell ref="G15:P15"/>
     <mergeCell ref="AG8:AL8"/>
     <mergeCell ref="AW6:BD6"/>
@@ -7598,65 +7677,6 @@
     <mergeCell ref="CI8:CN8"/>
     <mergeCell ref="CO8:CT8"/>
     <mergeCell ref="AM8:AR8"/>
-    <mergeCell ref="AS8:AX8"/>
-    <mergeCell ref="AY8:BD8"/>
-    <mergeCell ref="BE8:BJ8"/>
-    <mergeCell ref="BK8:BP8"/>
-    <mergeCell ref="BQ8:BV8"/>
-    <mergeCell ref="AK9:AL9"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="S9:T9"/>
-    <mergeCell ref="U9:V9"/>
-    <mergeCell ref="Y9:Z9"/>
-    <mergeCell ref="AA9:AB9"/>
-    <mergeCell ref="AE9:AF9"/>
-    <mergeCell ref="AG9:AH9"/>
-    <mergeCell ref="BE9:BF9"/>
-    <mergeCell ref="BI9:BJ9"/>
-    <mergeCell ref="BK9:BL9"/>
-    <mergeCell ref="BO9:BP9"/>
-    <mergeCell ref="BQ9:BR9"/>
-    <mergeCell ref="AQ9:AR9"/>
-    <mergeCell ref="AS9:AT9"/>
-    <mergeCell ref="AW9:AX9"/>
-    <mergeCell ref="AY9:AZ9"/>
-    <mergeCell ref="BC9:BD9"/>
-    <mergeCell ref="I3:V3"/>
-    <mergeCell ref="W3:AH3"/>
-    <mergeCell ref="AI3:BP3"/>
-    <mergeCell ref="BQ3:CH3"/>
-    <mergeCell ref="AJ37:BP37"/>
-    <mergeCell ref="AS24:AX24"/>
-    <mergeCell ref="AI23:AJ23"/>
-    <mergeCell ref="AI26:AK26"/>
-    <mergeCell ref="AI28:AK28"/>
-    <mergeCell ref="AW27:AY27"/>
-    <mergeCell ref="AW5:AZ5"/>
-    <mergeCell ref="AJ34:AZ34"/>
-    <mergeCell ref="Q18:Y18"/>
-    <mergeCell ref="AA20:AC20"/>
-    <mergeCell ref="Y23:AH23"/>
-    <mergeCell ref="AA25:AH25"/>
-    <mergeCell ref="CR6:DE6"/>
-    <mergeCell ref="BK38:BR38"/>
-    <mergeCell ref="AT38:AY38"/>
-    <mergeCell ref="BT41:BU41"/>
-    <mergeCell ref="BU42:CH42"/>
-    <mergeCell ref="AJ32:AW32"/>
-    <mergeCell ref="CO9:CP9"/>
-    <mergeCell ref="CS9:CT9"/>
-    <mergeCell ref="BW9:BX9"/>
-    <mergeCell ref="CA9:CB9"/>
-    <mergeCell ref="CC9:CD9"/>
-    <mergeCell ref="CG9:CH9"/>
-    <mergeCell ref="CI9:CJ9"/>
-    <mergeCell ref="CM9:CN9"/>
-    <mergeCell ref="BU9:BV9"/>
-    <mergeCell ref="AM9:AN9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
created pdfs in SoftwareManagement
</commit_message>
<xml_diff>
--- a/doc/SoftwareManagement/Projektplan.xlsx
+++ b/doc/SoftwareManagement/Projektplan.xlsx
@@ -1048,42 +1048,92 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="22" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="22" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="21" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="21" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="164" fontId="4" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="13" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="21" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1093,78 +1143,28 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="13" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="21" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="22" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="22" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="21" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="21" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1775,6 +1775,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:DO56"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
@@ -1830,114 +1833,114 @@
     <row r="3" spans="1:119" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
-      <c r="C3" s="137" t="s">
+      <c r="C3" s="164" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="137"/>
-      <c r="E3" s="137"/>
-      <c r="F3" s="137"/>
-      <c r="G3" s="137"/>
-      <c r="H3" s="137"/>
-      <c r="I3" s="145" t="s">
+      <c r="D3" s="164"/>
+      <c r="E3" s="164"/>
+      <c r="F3" s="164"/>
+      <c r="G3" s="164"/>
+      <c r="H3" s="164"/>
+      <c r="I3" s="139" t="s">
         <v>78</v>
       </c>
-      <c r="J3" s="145"/>
-      <c r="K3" s="145"/>
-      <c r="L3" s="145"/>
-      <c r="M3" s="145"/>
-      <c r="N3" s="145"/>
-      <c r="O3" s="145"/>
-      <c r="P3" s="145"/>
-      <c r="Q3" s="145"/>
-      <c r="R3" s="145"/>
-      <c r="S3" s="145"/>
-      <c r="T3" s="145"/>
-      <c r="U3" s="145"/>
-      <c r="V3" s="145"/>
-      <c r="W3" s="146" t="s">
+      <c r="J3" s="139"/>
+      <c r="K3" s="139"/>
+      <c r="L3" s="139"/>
+      <c r="M3" s="139"/>
+      <c r="N3" s="139"/>
+      <c r="O3" s="139"/>
+      <c r="P3" s="139"/>
+      <c r="Q3" s="139"/>
+      <c r="R3" s="139"/>
+      <c r="S3" s="139"/>
+      <c r="T3" s="139"/>
+      <c r="U3" s="139"/>
+      <c r="V3" s="139"/>
+      <c r="W3" s="140" t="s">
         <v>77</v>
       </c>
-      <c r="X3" s="146"/>
-      <c r="Y3" s="146"/>
-      <c r="Z3" s="146"/>
-      <c r="AA3" s="146"/>
-      <c r="AB3" s="146"/>
-      <c r="AC3" s="146"/>
-      <c r="AD3" s="146"/>
-      <c r="AE3" s="146"/>
-      <c r="AF3" s="146"/>
-      <c r="AG3" s="146"/>
-      <c r="AH3" s="146"/>
-      <c r="AI3" s="136" t="s">
+      <c r="X3" s="140"/>
+      <c r="Y3" s="140"/>
+      <c r="Z3" s="140"/>
+      <c r="AA3" s="140"/>
+      <c r="AB3" s="140"/>
+      <c r="AC3" s="140"/>
+      <c r="AD3" s="140"/>
+      <c r="AE3" s="140"/>
+      <c r="AF3" s="140"/>
+      <c r="AG3" s="140"/>
+      <c r="AH3" s="140"/>
+      <c r="AI3" s="141" t="s">
         <v>76</v>
       </c>
-      <c r="AJ3" s="136"/>
-      <c r="AK3" s="136"/>
-      <c r="AL3" s="136"/>
-      <c r="AM3" s="136"/>
-      <c r="AN3" s="136"/>
-      <c r="AO3" s="136"/>
-      <c r="AP3" s="136"/>
-      <c r="AQ3" s="136"/>
-      <c r="AR3" s="136"/>
-      <c r="AS3" s="136"/>
-      <c r="AT3" s="136"/>
-      <c r="AU3" s="136"/>
-      <c r="AV3" s="136"/>
-      <c r="AW3" s="136"/>
-      <c r="AX3" s="136"/>
-      <c r="AY3" s="136"/>
-      <c r="AZ3" s="136"/>
-      <c r="BA3" s="136"/>
-      <c r="BB3" s="136"/>
-      <c r="BC3" s="136"/>
-      <c r="BD3" s="136"/>
-      <c r="BE3" s="136"/>
-      <c r="BF3" s="136"/>
-      <c r="BG3" s="136"/>
-      <c r="BH3" s="136"/>
-      <c r="BI3" s="136"/>
-      <c r="BJ3" s="136"/>
-      <c r="BK3" s="136"/>
-      <c r="BL3" s="136"/>
-      <c r="BM3" s="136"/>
-      <c r="BN3" s="136"/>
-      <c r="BO3" s="136"/>
-      <c r="BP3" s="136"/>
-      <c r="BQ3" s="146" t="s">
+      <c r="AJ3" s="141"/>
+      <c r="AK3" s="141"/>
+      <c r="AL3" s="141"/>
+      <c r="AM3" s="141"/>
+      <c r="AN3" s="141"/>
+      <c r="AO3" s="141"/>
+      <c r="AP3" s="141"/>
+      <c r="AQ3" s="141"/>
+      <c r="AR3" s="141"/>
+      <c r="AS3" s="141"/>
+      <c r="AT3" s="141"/>
+      <c r="AU3" s="141"/>
+      <c r="AV3" s="141"/>
+      <c r="AW3" s="141"/>
+      <c r="AX3" s="141"/>
+      <c r="AY3" s="141"/>
+      <c r="AZ3" s="141"/>
+      <c r="BA3" s="141"/>
+      <c r="BB3" s="141"/>
+      <c r="BC3" s="141"/>
+      <c r="BD3" s="141"/>
+      <c r="BE3" s="141"/>
+      <c r="BF3" s="141"/>
+      <c r="BG3" s="141"/>
+      <c r="BH3" s="141"/>
+      <c r="BI3" s="141"/>
+      <c r="BJ3" s="141"/>
+      <c r="BK3" s="141"/>
+      <c r="BL3" s="141"/>
+      <c r="BM3" s="141"/>
+      <c r="BN3" s="141"/>
+      <c r="BO3" s="141"/>
+      <c r="BP3" s="141"/>
+      <c r="BQ3" s="140" t="s">
         <v>75</v>
       </c>
-      <c r="BR3" s="146"/>
-      <c r="BS3" s="146"/>
-      <c r="BT3" s="146"/>
-      <c r="BU3" s="146"/>
-      <c r="BV3" s="146"/>
-      <c r="BW3" s="146"/>
-      <c r="BX3" s="146"/>
-      <c r="BY3" s="146"/>
-      <c r="BZ3" s="146"/>
-      <c r="CA3" s="146"/>
-      <c r="CB3" s="146"/>
-      <c r="CC3" s="146"/>
-      <c r="CD3" s="146"/>
-      <c r="CE3" s="146"/>
-      <c r="CF3" s="146"/>
-      <c r="CG3" s="146"/>
-      <c r="CH3" s="146"/>
-      <c r="CI3" s="136" t="s">
+      <c r="BR3" s="140"/>
+      <c r="BS3" s="140"/>
+      <c r="BT3" s="140"/>
+      <c r="BU3" s="140"/>
+      <c r="BV3" s="140"/>
+      <c r="BW3" s="140"/>
+      <c r="BX3" s="140"/>
+      <c r="BY3" s="140"/>
+      <c r="BZ3" s="140"/>
+      <c r="CA3" s="140"/>
+      <c r="CB3" s="140"/>
+      <c r="CC3" s="140"/>
+      <c r="CD3" s="140"/>
+      <c r="CE3" s="140"/>
+      <c r="CF3" s="140"/>
+      <c r="CG3" s="140"/>
+      <c r="CH3" s="140"/>
+      <c r="CI3" s="141" t="s">
         <v>82</v>
       </c>
-      <c r="CJ3" s="136"/>
-      <c r="CK3" s="136"/>
-      <c r="CL3" s="136"/>
-      <c r="CM3" s="136"/>
-      <c r="CN3" s="136"/>
-      <c r="CO3" s="136"/>
-      <c r="CP3" s="136"/>
-      <c r="CQ3" s="136"/>
-      <c r="CR3" s="136"/>
-      <c r="CS3" s="136"/>
-      <c r="CT3" s="136"/>
+      <c r="CJ3" s="141"/>
+      <c r="CK3" s="141"/>
+      <c r="CL3" s="141"/>
+      <c r="CM3" s="141"/>
+      <c r="CN3" s="141"/>
+      <c r="CO3" s="141"/>
+      <c r="CP3" s="141"/>
+      <c r="CQ3" s="141"/>
+      <c r="CR3" s="141"/>
+      <c r="CS3" s="141"/>
+      <c r="CT3" s="141"/>
       <c r="CU3" s="60"/>
       <c r="CV3" s="60"/>
       <c r="CW3" s="60"/>
@@ -2106,12 +2109,12 @@
       <c r="AT5" s="23"/>
       <c r="AU5" s="23"/>
       <c r="AV5" s="23"/>
-      <c r="AW5" s="154" t="s">
+      <c r="AW5" s="149" t="s">
         <v>48</v>
       </c>
-      <c r="AX5" s="154"/>
-      <c r="AY5" s="154"/>
-      <c r="AZ5" s="154"/>
+      <c r="AX5" s="149"/>
+      <c r="AY5" s="149"/>
+      <c r="AZ5" s="149"/>
       <c r="BA5" s="23"/>
       <c r="BB5" s="23"/>
       <c r="BD5" s="23"/>
@@ -2181,14 +2184,14 @@
       <c r="Q6" s="22"/>
       <c r="T6" s="62"/>
       <c r="V6" s="23"/>
-      <c r="AA6" s="134" t="s">
+      <c r="AA6" s="162" t="s">
         <v>81</v>
       </c>
-      <c r="AB6" s="135"/>
-      <c r="AC6" s="135"/>
-      <c r="AD6" s="135"/>
-      <c r="AE6" s="135"/>
-      <c r="AF6" s="135"/>
+      <c r="AB6" s="163"/>
+      <c r="AC6" s="163"/>
+      <c r="AD6" s="163"/>
+      <c r="AE6" s="163"/>
+      <c r="AF6" s="163"/>
       <c r="AH6" s="23"/>
       <c r="AI6" s="62"/>
       <c r="AJ6" s="62"/>
@@ -2201,16 +2204,16 @@
       <c r="AT6" s="23"/>
       <c r="AU6" s="62"/>
       <c r="AV6" s="62"/>
-      <c r="AW6" s="132" t="s">
+      <c r="AW6" s="160" t="s">
         <v>80</v>
       </c>
-      <c r="AX6" s="133"/>
-      <c r="AY6" s="133"/>
-      <c r="AZ6" s="133"/>
-      <c r="BA6" s="133"/>
-      <c r="BB6" s="133"/>
-      <c r="BC6" s="133"/>
-      <c r="BD6" s="133"/>
+      <c r="AX6" s="161"/>
+      <c r="AY6" s="161"/>
+      <c r="AZ6" s="161"/>
+      <c r="BA6" s="161"/>
+      <c r="BB6" s="161"/>
+      <c r="BC6" s="161"/>
+      <c r="BD6" s="161"/>
       <c r="BF6" s="23"/>
       <c r="BG6" s="23"/>
       <c r="BH6" s="23"/>
@@ -2245,22 +2248,22 @@
       <c r="CL6" s="23"/>
       <c r="CP6" s="23"/>
       <c r="CQ6" s="23"/>
-      <c r="CR6" s="158" t="s">
+      <c r="CR6" s="128" t="s">
         <v>85</v>
       </c>
-      <c r="CS6" s="159"/>
-      <c r="CT6" s="159"/>
-      <c r="CU6" s="159"/>
-      <c r="CV6" s="159"/>
-      <c r="CW6" s="159"/>
-      <c r="CX6" s="159"/>
-      <c r="CY6" s="159"/>
-      <c r="CZ6" s="159"/>
-      <c r="DA6" s="159"/>
-      <c r="DB6" s="159"/>
-      <c r="DC6" s="159"/>
-      <c r="DD6" s="159"/>
-      <c r="DE6" s="159"/>
+      <c r="CS6" s="129"/>
+      <c r="CT6" s="129"/>
+      <c r="CU6" s="129"/>
+      <c r="CV6" s="129"/>
+      <c r="CW6" s="129"/>
+      <c r="CX6" s="129"/>
+      <c r="CY6" s="129"/>
+      <c r="CZ6" s="129"/>
+      <c r="DA6" s="129"/>
+      <c r="DB6" s="129"/>
+      <c r="DC6" s="129"/>
+      <c r="DD6" s="129"/>
+      <c r="DE6" s="129"/>
       <c r="DF6" s="23"/>
       <c r="DG6" s="23"/>
       <c r="DH6" s="23"/>
@@ -2358,134 +2361,134 @@
       <c r="DH7" s="23"/>
     </row>
     <row r="8" spans="1:119" x14ac:dyDescent="0.2">
-      <c r="C8" s="129" t="s">
+      <c r="C8" s="157" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="130"/>
-      <c r="E8" s="130"/>
-      <c r="F8" s="130"/>
-      <c r="G8" s="130"/>
-      <c r="H8" s="131"/>
-      <c r="I8" s="129" t="s">
+      <c r="D8" s="158"/>
+      <c r="E8" s="158"/>
+      <c r="F8" s="158"/>
+      <c r="G8" s="158"/>
+      <c r="H8" s="159"/>
+      <c r="I8" s="157" t="s">
         <v>14</v>
       </c>
-      <c r="J8" s="130"/>
-      <c r="K8" s="130"/>
-      <c r="L8" s="130"/>
-      <c r="M8" s="130"/>
-      <c r="N8" s="131"/>
-      <c r="O8" s="129" t="s">
+      <c r="J8" s="158"/>
+      <c r="K8" s="158"/>
+      <c r="L8" s="158"/>
+      <c r="M8" s="158"/>
+      <c r="N8" s="159"/>
+      <c r="O8" s="157" t="s">
         <v>15</v>
       </c>
-      <c r="P8" s="130"/>
-      <c r="Q8" s="130"/>
-      <c r="R8" s="130"/>
-      <c r="S8" s="130"/>
-      <c r="T8" s="131"/>
-      <c r="U8" s="129" t="s">
+      <c r="P8" s="158"/>
+      <c r="Q8" s="158"/>
+      <c r="R8" s="158"/>
+      <c r="S8" s="158"/>
+      <c r="T8" s="159"/>
+      <c r="U8" s="157" t="s">
         <v>16</v>
       </c>
-      <c r="V8" s="130"/>
-      <c r="W8" s="130"/>
-      <c r="X8" s="130"/>
-      <c r="Y8" s="130"/>
-      <c r="Z8" s="131"/>
-      <c r="AA8" s="129" t="s">
+      <c r="V8" s="158"/>
+      <c r="W8" s="158"/>
+      <c r="X8" s="158"/>
+      <c r="Y8" s="158"/>
+      <c r="Z8" s="159"/>
+      <c r="AA8" s="157" t="s">
         <v>17</v>
       </c>
-      <c r="AB8" s="130"/>
-      <c r="AC8" s="130"/>
-      <c r="AD8" s="130"/>
-      <c r="AE8" s="130"/>
-      <c r="AF8" s="131"/>
-      <c r="AG8" s="129" t="s">
+      <c r="AB8" s="158"/>
+      <c r="AC8" s="158"/>
+      <c r="AD8" s="158"/>
+      <c r="AE8" s="158"/>
+      <c r="AF8" s="159"/>
+      <c r="AG8" s="157" t="s">
         <v>18</v>
       </c>
-      <c r="AH8" s="130"/>
-      <c r="AI8" s="130"/>
-      <c r="AJ8" s="130"/>
-      <c r="AK8" s="130"/>
-      <c r="AL8" s="131"/>
-      <c r="AM8" s="129" t="s">
+      <c r="AH8" s="158"/>
+      <c r="AI8" s="158"/>
+      <c r="AJ8" s="158"/>
+      <c r="AK8" s="158"/>
+      <c r="AL8" s="159"/>
+      <c r="AM8" s="157" t="s">
         <v>19</v>
       </c>
-      <c r="AN8" s="130"/>
-      <c r="AO8" s="130"/>
-      <c r="AP8" s="130"/>
-      <c r="AQ8" s="130"/>
-      <c r="AR8" s="131"/>
-      <c r="AS8" s="129" t="s">
+      <c r="AN8" s="158"/>
+      <c r="AO8" s="158"/>
+      <c r="AP8" s="158"/>
+      <c r="AQ8" s="158"/>
+      <c r="AR8" s="159"/>
+      <c r="AS8" s="157" t="s">
         <v>20</v>
       </c>
-      <c r="AT8" s="130"/>
-      <c r="AU8" s="130"/>
-      <c r="AV8" s="130"/>
-      <c r="AW8" s="130"/>
-      <c r="AX8" s="131"/>
-      <c r="AY8" s="129" t="s">
+      <c r="AT8" s="158"/>
+      <c r="AU8" s="158"/>
+      <c r="AV8" s="158"/>
+      <c r="AW8" s="158"/>
+      <c r="AX8" s="159"/>
+      <c r="AY8" s="157" t="s">
         <v>21</v>
       </c>
-      <c r="AZ8" s="130"/>
-      <c r="BA8" s="130"/>
-      <c r="BB8" s="130"/>
-      <c r="BC8" s="130"/>
-      <c r="BD8" s="131"/>
-      <c r="BE8" s="129" t="s">
+      <c r="AZ8" s="158"/>
+      <c r="BA8" s="158"/>
+      <c r="BB8" s="158"/>
+      <c r="BC8" s="158"/>
+      <c r="BD8" s="159"/>
+      <c r="BE8" s="157" t="s">
         <v>22</v>
       </c>
-      <c r="BF8" s="130"/>
-      <c r="BG8" s="130"/>
-      <c r="BH8" s="130"/>
-      <c r="BI8" s="130"/>
-      <c r="BJ8" s="131"/>
-      <c r="BK8" s="129" t="s">
+      <c r="BF8" s="158"/>
+      <c r="BG8" s="158"/>
+      <c r="BH8" s="158"/>
+      <c r="BI8" s="158"/>
+      <c r="BJ8" s="159"/>
+      <c r="BK8" s="157" t="s">
         <v>23</v>
       </c>
-      <c r="BL8" s="130"/>
-      <c r="BM8" s="130"/>
-      <c r="BN8" s="130"/>
-      <c r="BO8" s="130"/>
-      <c r="BP8" s="131"/>
-      <c r="BQ8" s="129" t="s">
+      <c r="BL8" s="158"/>
+      <c r="BM8" s="158"/>
+      <c r="BN8" s="158"/>
+      <c r="BO8" s="158"/>
+      <c r="BP8" s="159"/>
+      <c r="BQ8" s="157" t="s">
         <v>24</v>
       </c>
-      <c r="BR8" s="130"/>
-      <c r="BS8" s="130"/>
-      <c r="BT8" s="130"/>
-      <c r="BU8" s="130"/>
-      <c r="BV8" s="131"/>
-      <c r="BW8" s="129" t="s">
+      <c r="BR8" s="158"/>
+      <c r="BS8" s="158"/>
+      <c r="BT8" s="158"/>
+      <c r="BU8" s="158"/>
+      <c r="BV8" s="159"/>
+      <c r="BW8" s="157" t="s">
         <v>25</v>
       </c>
-      <c r="BX8" s="130"/>
-      <c r="BY8" s="130"/>
-      <c r="BZ8" s="130"/>
-      <c r="CA8" s="130"/>
-      <c r="CB8" s="131"/>
-      <c r="CC8" s="129" t="s">
+      <c r="BX8" s="158"/>
+      <c r="BY8" s="158"/>
+      <c r="BZ8" s="158"/>
+      <c r="CA8" s="158"/>
+      <c r="CB8" s="159"/>
+      <c r="CC8" s="157" t="s">
         <v>5</v>
       </c>
-      <c r="CD8" s="130"/>
-      <c r="CE8" s="130"/>
-      <c r="CF8" s="130"/>
-      <c r="CG8" s="130"/>
-      <c r="CH8" s="131"/>
-      <c r="CI8" s="129" t="s">
+      <c r="CD8" s="158"/>
+      <c r="CE8" s="158"/>
+      <c r="CF8" s="158"/>
+      <c r="CG8" s="158"/>
+      <c r="CH8" s="159"/>
+      <c r="CI8" s="157" t="s">
         <v>6</v>
       </c>
-      <c r="CJ8" s="130"/>
-      <c r="CK8" s="130"/>
-      <c r="CL8" s="130"/>
-      <c r="CM8" s="130"/>
-      <c r="CN8" s="131"/>
-      <c r="CO8" s="129" t="s">
+      <c r="CJ8" s="158"/>
+      <c r="CK8" s="158"/>
+      <c r="CL8" s="158"/>
+      <c r="CM8" s="158"/>
+      <c r="CN8" s="159"/>
+      <c r="CO8" s="157" t="s">
         <v>7</v>
       </c>
-      <c r="CP8" s="130"/>
-      <c r="CQ8" s="130"/>
-      <c r="CR8" s="130"/>
-      <c r="CS8" s="130"/>
-      <c r="CT8" s="131"/>
+      <c r="CP8" s="158"/>
+      <c r="CQ8" s="158"/>
+      <c r="CR8" s="158"/>
+      <c r="CS8" s="158"/>
+      <c r="CT8" s="159"/>
       <c r="CV8" s="80"/>
       <c r="CW8" s="80"/>
       <c r="CX8" s="80"/>
@@ -2505,195 +2508,195 @@
         <v>27</v>
       </c>
       <c r="B9" s="15"/>
-      <c r="C9" s="140" t="s">
+      <c r="C9" s="153" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="141"/>
+      <c r="D9" s="154"/>
       <c r="E9" s="69"/>
       <c r="F9" s="69"/>
-      <c r="G9" s="142" t="s">
+      <c r="G9" s="155" t="s">
         <v>28</v>
       </c>
-      <c r="H9" s="143"/>
-      <c r="I9" s="144">
+      <c r="H9" s="156"/>
+      <c r="I9" s="136">
         <v>40959</v>
       </c>
-      <c r="J9" s="141"/>
+      <c r="J9" s="154"/>
       <c r="K9" s="69"/>
       <c r="L9" s="69"/>
-      <c r="M9" s="138">
+      <c r="M9" s="137">
         <f>SUM(I9+6)</f>
         <v>40965</v>
       </c>
-      <c r="N9" s="139"/>
-      <c r="O9" s="144">
+      <c r="N9" s="138"/>
+      <c r="O9" s="136">
         <f>SUM(M9+1)</f>
         <v>40966</v>
       </c>
-      <c r="P9" s="138"/>
+      <c r="P9" s="137"/>
       <c r="Q9" s="70"/>
       <c r="R9" s="70"/>
-      <c r="S9" s="138">
+      <c r="S9" s="137">
         <f>SUM(O9+6)</f>
         <v>40972</v>
       </c>
-      <c r="T9" s="139"/>
-      <c r="U9" s="144">
+      <c r="T9" s="138"/>
+      <c r="U9" s="136">
         <f>SUM(S9+1)</f>
         <v>40973</v>
       </c>
-      <c r="V9" s="138"/>
+      <c r="V9" s="137"/>
       <c r="W9" s="70"/>
       <c r="X9" s="70"/>
-      <c r="Y9" s="138">
+      <c r="Y9" s="137">
         <f>SUM(U9+6)</f>
         <v>40979</v>
       </c>
-      <c r="Z9" s="139"/>
-      <c r="AA9" s="144">
+      <c r="Z9" s="138"/>
+      <c r="AA9" s="136">
         <f>SUM(Y9+1)</f>
         <v>40980</v>
       </c>
-      <c r="AB9" s="138"/>
+      <c r="AB9" s="137"/>
       <c r="AC9" s="70"/>
       <c r="AD9" s="70"/>
-      <c r="AE9" s="138">
+      <c r="AE9" s="137">
         <f>SUM(AA9+6)</f>
         <v>40986</v>
       </c>
-      <c r="AF9" s="139"/>
-      <c r="AG9" s="144">
+      <c r="AF9" s="138"/>
+      <c r="AG9" s="136">
         <f>SUM(AE9+1)</f>
         <v>40987</v>
       </c>
-      <c r="AH9" s="138"/>
+      <c r="AH9" s="137"/>
       <c r="AI9" s="70"/>
       <c r="AJ9" s="70"/>
-      <c r="AK9" s="138">
+      <c r="AK9" s="137">
         <f>SUM(AG9+6)</f>
         <v>40993</v>
       </c>
-      <c r="AL9" s="139"/>
-      <c r="AM9" s="144">
+      <c r="AL9" s="138"/>
+      <c r="AM9" s="136">
         <f>SUM(AK9+1)</f>
         <v>40994</v>
       </c>
-      <c r="AN9" s="138"/>
+      <c r="AN9" s="137"/>
       <c r="AO9" s="70"/>
       <c r="AP9" s="70"/>
-      <c r="AQ9" s="138">
+      <c r="AQ9" s="137">
         <f>SUM(AM9+6)</f>
         <v>41000</v>
       </c>
-      <c r="AR9" s="139"/>
-      <c r="AS9" s="144">
+      <c r="AR9" s="138"/>
+      <c r="AS9" s="136">
         <f>SUM(AQ9+1)</f>
         <v>41001</v>
       </c>
-      <c r="AT9" s="138"/>
+      <c r="AT9" s="137"/>
       <c r="AU9" s="70"/>
       <c r="AV9" s="70"/>
-      <c r="AW9" s="138">
+      <c r="AW9" s="137">
         <f>SUM(AS9+6)</f>
         <v>41007</v>
       </c>
-      <c r="AX9" s="139"/>
-      <c r="AY9" s="144">
+      <c r="AX9" s="138"/>
+      <c r="AY9" s="136">
         <f>SUM(AW9+1)</f>
         <v>41008</v>
       </c>
-      <c r="AZ9" s="138"/>
+      <c r="AZ9" s="137"/>
       <c r="BA9" s="70"/>
       <c r="BB9" s="70"/>
-      <c r="BC9" s="138">
+      <c r="BC9" s="137">
         <f>SUM(AY9+6)</f>
         <v>41014</v>
       </c>
-      <c r="BD9" s="139"/>
-      <c r="BE9" s="144">
+      <c r="BD9" s="138"/>
+      <c r="BE9" s="136">
         <f>SUM(BC9+1)</f>
         <v>41015</v>
       </c>
-      <c r="BF9" s="138"/>
+      <c r="BF9" s="137"/>
       <c r="BG9" s="70"/>
       <c r="BH9" s="70"/>
-      <c r="BI9" s="138">
+      <c r="BI9" s="137">
         <f>SUM(BE9+6)</f>
         <v>41021</v>
       </c>
-      <c r="BJ9" s="139"/>
-      <c r="BK9" s="144">
+      <c r="BJ9" s="138"/>
+      <c r="BK9" s="136">
         <f>SUM(BI9+1)</f>
         <v>41022</v>
       </c>
-      <c r="BL9" s="138"/>
+      <c r="BL9" s="137"/>
       <c r="BM9" s="70"/>
       <c r="BN9" s="70"/>
-      <c r="BO9" s="138">
+      <c r="BO9" s="137">
         <f>SUM(BK9+6)</f>
         <v>41028</v>
       </c>
-      <c r="BP9" s="139"/>
-      <c r="BQ9" s="144">
+      <c r="BP9" s="138"/>
+      <c r="BQ9" s="136">
         <f>SUM(BO9+1)</f>
         <v>41029</v>
       </c>
-      <c r="BR9" s="138"/>
+      <c r="BR9" s="137"/>
       <c r="BS9" s="70"/>
       <c r="BT9" s="70"/>
-      <c r="BU9" s="138">
+      <c r="BU9" s="137">
         <f>SUM(BQ9+6)</f>
         <v>41035</v>
       </c>
-      <c r="BV9" s="139"/>
-      <c r="BW9" s="144">
+      <c r="BV9" s="138"/>
+      <c r="BW9" s="136">
         <f>SUM(BU9+1)</f>
         <v>41036</v>
       </c>
-      <c r="BX9" s="138"/>
+      <c r="BX9" s="137"/>
       <c r="BY9" s="70"/>
       <c r="BZ9" s="70"/>
-      <c r="CA9" s="138">
+      <c r="CA9" s="137">
         <f>SUM(BW9+6)</f>
         <v>41042</v>
       </c>
-      <c r="CB9" s="139"/>
-      <c r="CC9" s="144">
+      <c r="CB9" s="138"/>
+      <c r="CC9" s="136">
         <f>SUM(CA9+1)</f>
         <v>41043</v>
       </c>
-      <c r="CD9" s="138"/>
+      <c r="CD9" s="137"/>
       <c r="CE9" s="70"/>
       <c r="CF9" s="70"/>
-      <c r="CG9" s="138">
+      <c r="CG9" s="137">
         <f>SUM(CC9+6)</f>
         <v>41049</v>
       </c>
-      <c r="CH9" s="139"/>
-      <c r="CI9" s="144">
+      <c r="CH9" s="138"/>
+      <c r="CI9" s="136">
         <f>SUM(CG9+1)</f>
         <v>41050</v>
       </c>
-      <c r="CJ9" s="138"/>
+      <c r="CJ9" s="137"/>
       <c r="CK9" s="70"/>
       <c r="CL9" s="70"/>
-      <c r="CM9" s="138">
+      <c r="CM9" s="137">
         <f>SUM(CI9+6)</f>
         <v>41056</v>
       </c>
-      <c r="CN9" s="139"/>
-      <c r="CO9" s="144">
+      <c r="CN9" s="138"/>
+      <c r="CO9" s="136">
         <f>SUM(CM9+1)</f>
         <v>41057</v>
       </c>
-      <c r="CP9" s="138"/>
+      <c r="CP9" s="137"/>
       <c r="CQ9" s="70"/>
       <c r="CR9" s="70"/>
-      <c r="CS9" s="138">
+      <c r="CS9" s="137">
         <f>SUM(CO9+6)</f>
         <v>41063</v>
       </c>
-      <c r="CT9" s="139"/>
+      <c r="CT9" s="138"/>
       <c r="CV9" s="62"/>
       <c r="CW9" s="62"/>
       <c r="CX9" s="68"/>
@@ -3289,16 +3292,16 @@
       <c r="D15" s="25"/>
       <c r="E15" s="25"/>
       <c r="F15" s="25"/>
-      <c r="G15" s="128"/>
-      <c r="H15" s="128"/>
-      <c r="I15" s="128"/>
-      <c r="J15" s="128"/>
-      <c r="K15" s="128"/>
-      <c r="L15" s="128"/>
-      <c r="M15" s="128"/>
-      <c r="N15" s="128"/>
-      <c r="O15" s="128"/>
-      <c r="P15" s="128"/>
+      <c r="G15" s="133"/>
+      <c r="H15" s="133"/>
+      <c r="I15" s="133"/>
+      <c r="J15" s="133"/>
+      <c r="K15" s="133"/>
+      <c r="L15" s="133"/>
+      <c r="M15" s="133"/>
+      <c r="N15" s="133"/>
+      <c r="O15" s="133"/>
+      <c r="P15" s="133"/>
       <c r="Q15" s="25"/>
       <c r="R15" s="25"/>
       <c r="S15" s="26"/>
@@ -3644,15 +3647,15 @@
       <c r="N18" s="27"/>
       <c r="O18" s="24"/>
       <c r="P18" s="25"/>
-      <c r="Q18" s="156"/>
-      <c r="R18" s="156"/>
-      <c r="S18" s="156"/>
-      <c r="T18" s="156"/>
-      <c r="U18" s="156"/>
-      <c r="V18" s="156"/>
-      <c r="W18" s="156"/>
-      <c r="X18" s="156"/>
-      <c r="Y18" s="156"/>
+      <c r="Q18" s="151"/>
+      <c r="R18" s="151"/>
+      <c r="S18" s="151"/>
+      <c r="T18" s="151"/>
+      <c r="U18" s="151"/>
+      <c r="V18" s="151"/>
+      <c r="W18" s="151"/>
+      <c r="X18" s="151"/>
+      <c r="Y18" s="151"/>
       <c r="Z18" s="27"/>
       <c r="AA18" s="24"/>
       <c r="AB18" s="25"/>
@@ -3886,9 +3889,9 @@
       <c r="X20" s="25"/>
       <c r="Y20" s="26"/>
       <c r="Z20" s="27"/>
-      <c r="AA20" s="157"/>
-      <c r="AB20" s="156"/>
-      <c r="AC20" s="156"/>
+      <c r="AA20" s="152"/>
+      <c r="AB20" s="151"/>
+      <c r="AC20" s="151"/>
       <c r="AD20" s="25"/>
       <c r="AE20" s="26"/>
       <c r="AF20" s="27"/>
@@ -4229,18 +4232,18 @@
       <c r="V23" s="25"/>
       <c r="W23" s="25"/>
       <c r="X23" s="25"/>
-      <c r="Y23" s="150"/>
-      <c r="Z23" s="150"/>
-      <c r="AA23" s="150"/>
-      <c r="AB23" s="150"/>
-      <c r="AC23" s="150"/>
-      <c r="AD23" s="150"/>
-      <c r="AE23" s="150"/>
-      <c r="AF23" s="150"/>
-      <c r="AG23" s="150"/>
-      <c r="AH23" s="150"/>
-      <c r="AI23" s="152"/>
-      <c r="AJ23" s="152"/>
+      <c r="Y23" s="145"/>
+      <c r="Z23" s="145"/>
+      <c r="AA23" s="145"/>
+      <c r="AB23" s="145"/>
+      <c r="AC23" s="145"/>
+      <c r="AD23" s="145"/>
+      <c r="AE23" s="145"/>
+      <c r="AF23" s="145"/>
+      <c r="AG23" s="145"/>
+      <c r="AH23" s="145"/>
+      <c r="AI23" s="147"/>
+      <c r="AJ23" s="147"/>
       <c r="AK23" s="26"/>
       <c r="AL23" s="27"/>
       <c r="AM23" s="24"/>
@@ -4359,12 +4362,12 @@
       <c r="AJ24" s="25"/>
       <c r="AK24" s="26"/>
       <c r="AL24" s="27"/>
-      <c r="AS24" s="149"/>
-      <c r="AT24" s="150"/>
-      <c r="AU24" s="150"/>
-      <c r="AV24" s="150"/>
-      <c r="AW24" s="150"/>
-      <c r="AX24" s="151"/>
+      <c r="AS24" s="144"/>
+      <c r="AT24" s="145"/>
+      <c r="AU24" s="145"/>
+      <c r="AV24" s="145"/>
+      <c r="AW24" s="145"/>
+      <c r="AX24" s="146"/>
       <c r="AY24" s="24"/>
       <c r="AZ24" s="25"/>
       <c r="BA24" s="26"/>
@@ -4457,14 +4460,14 @@
       <c r="X25" s="25"/>
       <c r="Y25" s="26"/>
       <c r="Z25" s="27"/>
-      <c r="AA25" s="149"/>
-      <c r="AB25" s="150"/>
-      <c r="AC25" s="150"/>
-      <c r="AD25" s="150"/>
-      <c r="AE25" s="150"/>
-      <c r="AF25" s="150"/>
-      <c r="AG25" s="150"/>
-      <c r="AH25" s="150"/>
+      <c r="AA25" s="144"/>
+      <c r="AB25" s="145"/>
+      <c r="AC25" s="145"/>
+      <c r="AD25" s="145"/>
+      <c r="AE25" s="145"/>
+      <c r="AF25" s="145"/>
+      <c r="AG25" s="145"/>
+      <c r="AH25" s="145"/>
       <c r="AI25" s="26"/>
       <c r="AJ25" s="25"/>
       <c r="AK25" s="26"/>
@@ -4581,9 +4584,9 @@
       <c r="AF26" s="27"/>
       <c r="AG26" s="24"/>
       <c r="AH26" s="25"/>
-      <c r="AI26" s="150"/>
-      <c r="AJ26" s="150"/>
-      <c r="AK26" s="150"/>
+      <c r="AI26" s="145"/>
+      <c r="AJ26" s="145"/>
+      <c r="AK26" s="145"/>
       <c r="AL26" s="27"/>
       <c r="AM26" s="24"/>
       <c r="AN26" s="25"/>
@@ -4700,9 +4703,9 @@
       <c r="AI27" s="26"/>
       <c r="AM27" s="113"/>
       <c r="AS27" s="113"/>
-      <c r="AW27" s="153"/>
-      <c r="AX27" s="153"/>
-      <c r="AY27" s="153"/>
+      <c r="AW27" s="148"/>
+      <c r="AX27" s="148"/>
+      <c r="AY27" s="148"/>
       <c r="BA27" s="26"/>
       <c r="BB27" s="25"/>
       <c r="BC27" s="26"/>
@@ -4801,9 +4804,9 @@
       <c r="AF28" s="27"/>
       <c r="AG28" s="24"/>
       <c r="AH28" s="25"/>
-      <c r="AI28" s="150"/>
-      <c r="AJ28" s="150"/>
-      <c r="AK28" s="150"/>
+      <c r="AI28" s="145"/>
+      <c r="AJ28" s="145"/>
+      <c r="AK28" s="145"/>
       <c r="AL28" s="27"/>
       <c r="AM28" s="24"/>
       <c r="AN28" s="25"/>
@@ -5251,20 +5254,20 @@
       <c r="AG32" s="24"/>
       <c r="AH32" s="25"/>
       <c r="AI32" s="26"/>
-      <c r="AJ32" s="164"/>
-      <c r="AK32" s="164"/>
-      <c r="AL32" s="164"/>
-      <c r="AM32" s="164"/>
-      <c r="AN32" s="164"/>
-      <c r="AO32" s="164"/>
-      <c r="AP32" s="164"/>
-      <c r="AQ32" s="164"/>
-      <c r="AR32" s="164"/>
-      <c r="AS32" s="164"/>
-      <c r="AT32" s="164"/>
-      <c r="AU32" s="164"/>
-      <c r="AV32" s="164"/>
-      <c r="AW32" s="164"/>
+      <c r="AJ32" s="135"/>
+      <c r="AK32" s="135"/>
+      <c r="AL32" s="135"/>
+      <c r="AM32" s="135"/>
+      <c r="AN32" s="135"/>
+      <c r="AO32" s="135"/>
+      <c r="AP32" s="135"/>
+      <c r="AQ32" s="135"/>
+      <c r="AR32" s="135"/>
+      <c r="AS32" s="135"/>
+      <c r="AT32" s="135"/>
+      <c r="AU32" s="135"/>
+      <c r="AV32" s="135"/>
+      <c r="AW32" s="135"/>
       <c r="AX32" s="27"/>
       <c r="AY32" s="24"/>
       <c r="AZ32" s="25"/>
@@ -5483,23 +5486,23 @@
       <c r="AG34" s="24"/>
       <c r="AH34" s="25"/>
       <c r="AI34" s="26"/>
-      <c r="AJ34" s="155"/>
-      <c r="AK34" s="155"/>
-      <c r="AL34" s="155"/>
-      <c r="AM34" s="155"/>
-      <c r="AN34" s="155"/>
-      <c r="AO34" s="155"/>
-      <c r="AP34" s="155"/>
-      <c r="AQ34" s="155"/>
-      <c r="AR34" s="155"/>
-      <c r="AS34" s="155"/>
-      <c r="AT34" s="155"/>
-      <c r="AU34" s="155"/>
-      <c r="AV34" s="155"/>
-      <c r="AW34" s="155"/>
-      <c r="AX34" s="155"/>
-      <c r="AY34" s="155"/>
-      <c r="AZ34" s="155"/>
+      <c r="AJ34" s="150"/>
+      <c r="AK34" s="150"/>
+      <c r="AL34" s="150"/>
+      <c r="AM34" s="150"/>
+      <c r="AN34" s="150"/>
+      <c r="AO34" s="150"/>
+      <c r="AP34" s="150"/>
+      <c r="AQ34" s="150"/>
+      <c r="AR34" s="150"/>
+      <c r="AS34" s="150"/>
+      <c r="AT34" s="150"/>
+      <c r="AU34" s="150"/>
+      <c r="AV34" s="150"/>
+      <c r="AW34" s="150"/>
+      <c r="AX34" s="150"/>
+      <c r="AY34" s="150"/>
+      <c r="AZ34" s="150"/>
       <c r="BA34" s="26"/>
       <c r="BB34" s="25"/>
       <c r="BC34" s="26"/>
@@ -5797,39 +5800,39 @@
       <c r="AG37" s="24"/>
       <c r="AH37" s="25"/>
       <c r="AI37" s="26"/>
-      <c r="AJ37" s="147"/>
-      <c r="AK37" s="147"/>
-      <c r="AL37" s="147"/>
-      <c r="AM37" s="147"/>
-      <c r="AN37" s="147"/>
-      <c r="AO37" s="147"/>
-      <c r="AP37" s="147"/>
-      <c r="AQ37" s="147"/>
-      <c r="AR37" s="147"/>
-      <c r="AS37" s="147"/>
-      <c r="AT37" s="147"/>
-      <c r="AU37" s="147"/>
-      <c r="AV37" s="147"/>
-      <c r="AW37" s="147"/>
-      <c r="AX37" s="147"/>
-      <c r="AY37" s="147"/>
-      <c r="AZ37" s="147"/>
-      <c r="BA37" s="147"/>
-      <c r="BB37" s="147"/>
-      <c r="BC37" s="147"/>
-      <c r="BD37" s="147"/>
-      <c r="BE37" s="147"/>
-      <c r="BF37" s="147"/>
-      <c r="BG37" s="147"/>
-      <c r="BH37" s="147"/>
-      <c r="BI37" s="147"/>
-      <c r="BJ37" s="147"/>
-      <c r="BK37" s="147"/>
-      <c r="BL37" s="147"/>
-      <c r="BM37" s="147"/>
-      <c r="BN37" s="147"/>
-      <c r="BO37" s="147"/>
-      <c r="BP37" s="148"/>
+      <c r="AJ37" s="142"/>
+      <c r="AK37" s="142"/>
+      <c r="AL37" s="142"/>
+      <c r="AM37" s="142"/>
+      <c r="AN37" s="142"/>
+      <c r="AO37" s="142"/>
+      <c r="AP37" s="142"/>
+      <c r="AQ37" s="142"/>
+      <c r="AR37" s="142"/>
+      <c r="AS37" s="142"/>
+      <c r="AT37" s="142"/>
+      <c r="AU37" s="142"/>
+      <c r="AV37" s="142"/>
+      <c r="AW37" s="142"/>
+      <c r="AX37" s="142"/>
+      <c r="AY37" s="142"/>
+      <c r="AZ37" s="142"/>
+      <c r="BA37" s="142"/>
+      <c r="BB37" s="142"/>
+      <c r="BC37" s="142"/>
+      <c r="BD37" s="142"/>
+      <c r="BE37" s="142"/>
+      <c r="BF37" s="142"/>
+      <c r="BG37" s="142"/>
+      <c r="BH37" s="142"/>
+      <c r="BI37" s="142"/>
+      <c r="BJ37" s="142"/>
+      <c r="BK37" s="142"/>
+      <c r="BL37" s="142"/>
+      <c r="BM37" s="142"/>
+      <c r="BN37" s="142"/>
+      <c r="BO37" s="142"/>
+      <c r="BP37" s="143"/>
       <c r="BQ37" s="83"/>
       <c r="BR37" s="84"/>
       <c r="BS37" s="85"/>
@@ -5923,12 +5926,12 @@
       <c r="AQ38" s="26"/>
       <c r="AR38" s="27"/>
       <c r="AS38" s="24"/>
-      <c r="AT38" s="161"/>
-      <c r="AU38" s="161"/>
-      <c r="AV38" s="161"/>
-      <c r="AW38" s="161"/>
-      <c r="AX38" s="161"/>
-      <c r="AY38" s="161"/>
+      <c r="AT38" s="131"/>
+      <c r="AU38" s="131"/>
+      <c r="AV38" s="131"/>
+      <c r="AW38" s="131"/>
+      <c r="AX38" s="131"/>
+      <c r="AY38" s="131"/>
       <c r="AZ38" s="25"/>
       <c r="BA38" s="26"/>
       <c r="BB38" s="25"/>
@@ -5940,14 +5943,14 @@
       <c r="BH38" s="120"/>
       <c r="BI38" s="120"/>
       <c r="BJ38" s="120"/>
-      <c r="BK38" s="160"/>
-      <c r="BL38" s="160"/>
-      <c r="BM38" s="160"/>
-      <c r="BN38" s="160"/>
-      <c r="BO38" s="160"/>
-      <c r="BP38" s="160"/>
-      <c r="BQ38" s="160"/>
-      <c r="BR38" s="160"/>
+      <c r="BK38" s="130"/>
+      <c r="BL38" s="130"/>
+      <c r="BM38" s="130"/>
+      <c r="BN38" s="130"/>
+      <c r="BO38" s="130"/>
+      <c r="BP38" s="130"/>
+      <c r="BQ38" s="130"/>
+      <c r="BR38" s="130"/>
       <c r="BS38" s="120"/>
       <c r="BT38" s="120"/>
       <c r="BU38" s="26"/>
@@ -6294,8 +6297,8 @@
       <c r="BQ41" s="24"/>
       <c r="BR41" s="25"/>
       <c r="BS41" s="26"/>
-      <c r="BT41" s="162"/>
-      <c r="BU41" s="162"/>
+      <c r="BT41" s="132"/>
+      <c r="BU41" s="132"/>
       <c r="BV41" s="27"/>
       <c r="BW41" s="24"/>
       <c r="BX41" s="25"/>
@@ -6411,20 +6414,20 @@
       <c r="BR42" s="25"/>
       <c r="BS42" s="26"/>
       <c r="BT42" s="25"/>
-      <c r="BU42" s="128"/>
-      <c r="BV42" s="128"/>
-      <c r="BW42" s="128"/>
-      <c r="BX42" s="128"/>
-      <c r="BY42" s="128"/>
-      <c r="BZ42" s="128"/>
-      <c r="CA42" s="128"/>
-      <c r="CB42" s="128"/>
-      <c r="CC42" s="128"/>
-      <c r="CD42" s="128"/>
-      <c r="CE42" s="128"/>
-      <c r="CF42" s="128"/>
-      <c r="CG42" s="128"/>
-      <c r="CH42" s="163"/>
+      <c r="BU42" s="133"/>
+      <c r="BV42" s="133"/>
+      <c r="BW42" s="133"/>
+      <c r="BX42" s="133"/>
+      <c r="BY42" s="133"/>
+      <c r="BZ42" s="133"/>
+      <c r="CA42" s="133"/>
+      <c r="CB42" s="133"/>
+      <c r="CC42" s="133"/>
+      <c r="CD42" s="133"/>
+      <c r="CE42" s="133"/>
+      <c r="CF42" s="133"/>
+      <c r="CG42" s="133"/>
+      <c r="CH42" s="134"/>
       <c r="CI42" s="24"/>
       <c r="CJ42" s="25"/>
       <c r="CK42" s="26"/>
@@ -7602,6 +7605,65 @@
     </row>
   </sheetData>
   <mergeCells count="75">
+    <mergeCell ref="G15:P15"/>
+    <mergeCell ref="AG8:AL8"/>
+    <mergeCell ref="AW6:BD6"/>
+    <mergeCell ref="AA6:AF6"/>
+    <mergeCell ref="CI3:CT3"/>
+    <mergeCell ref="C3:H3"/>
+    <mergeCell ref="C8:H8"/>
+    <mergeCell ref="I8:N8"/>
+    <mergeCell ref="O8:T8"/>
+    <mergeCell ref="U8:Z8"/>
+    <mergeCell ref="AA8:AF8"/>
+    <mergeCell ref="BW8:CB8"/>
+    <mergeCell ref="CC8:CH8"/>
+    <mergeCell ref="CI8:CN8"/>
+    <mergeCell ref="CO8:CT8"/>
+    <mergeCell ref="AM8:AR8"/>
+    <mergeCell ref="AS8:AX8"/>
+    <mergeCell ref="AY8:BD8"/>
+    <mergeCell ref="BE8:BJ8"/>
+    <mergeCell ref="BK8:BP8"/>
+    <mergeCell ref="BQ8:BV8"/>
+    <mergeCell ref="AK9:AL9"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="S9:T9"/>
+    <mergeCell ref="U9:V9"/>
+    <mergeCell ref="Y9:Z9"/>
+    <mergeCell ref="AA9:AB9"/>
+    <mergeCell ref="AE9:AF9"/>
+    <mergeCell ref="AG9:AH9"/>
+    <mergeCell ref="BE9:BF9"/>
+    <mergeCell ref="BI9:BJ9"/>
+    <mergeCell ref="BK9:BL9"/>
+    <mergeCell ref="BO9:BP9"/>
+    <mergeCell ref="BQ9:BR9"/>
+    <mergeCell ref="AQ9:AR9"/>
+    <mergeCell ref="AS9:AT9"/>
+    <mergeCell ref="AW9:AX9"/>
+    <mergeCell ref="AY9:AZ9"/>
+    <mergeCell ref="BC9:BD9"/>
+    <mergeCell ref="I3:V3"/>
+    <mergeCell ref="W3:AH3"/>
+    <mergeCell ref="AI3:BP3"/>
+    <mergeCell ref="BQ3:CH3"/>
+    <mergeCell ref="AJ37:BP37"/>
+    <mergeCell ref="AS24:AX24"/>
+    <mergeCell ref="AI23:AJ23"/>
+    <mergeCell ref="AI26:AK26"/>
+    <mergeCell ref="AI28:AK28"/>
+    <mergeCell ref="AW27:AY27"/>
+    <mergeCell ref="AW5:AZ5"/>
+    <mergeCell ref="AJ34:AZ34"/>
+    <mergeCell ref="Q18:Y18"/>
+    <mergeCell ref="AA20:AC20"/>
+    <mergeCell ref="Y23:AH23"/>
+    <mergeCell ref="AA25:AH25"/>
     <mergeCell ref="CR6:DE6"/>
     <mergeCell ref="BK38:BR38"/>
     <mergeCell ref="AT38:AY38"/>
@@ -7618,68 +7680,9 @@
     <mergeCell ref="CM9:CN9"/>
     <mergeCell ref="BU9:BV9"/>
     <mergeCell ref="AM9:AN9"/>
-    <mergeCell ref="I3:V3"/>
-    <mergeCell ref="W3:AH3"/>
-    <mergeCell ref="AI3:BP3"/>
-    <mergeCell ref="BQ3:CH3"/>
-    <mergeCell ref="AJ37:BP37"/>
-    <mergeCell ref="AS24:AX24"/>
-    <mergeCell ref="AI23:AJ23"/>
-    <mergeCell ref="AI26:AK26"/>
-    <mergeCell ref="AI28:AK28"/>
-    <mergeCell ref="AW27:AY27"/>
-    <mergeCell ref="AW5:AZ5"/>
-    <mergeCell ref="AJ34:AZ34"/>
-    <mergeCell ref="Q18:Y18"/>
-    <mergeCell ref="AA20:AC20"/>
-    <mergeCell ref="Y23:AH23"/>
-    <mergeCell ref="AA25:AH25"/>
-    <mergeCell ref="AQ9:AR9"/>
-    <mergeCell ref="AS9:AT9"/>
-    <mergeCell ref="AW9:AX9"/>
-    <mergeCell ref="AY9:AZ9"/>
-    <mergeCell ref="BC9:BD9"/>
-    <mergeCell ref="BE9:BF9"/>
-    <mergeCell ref="BI9:BJ9"/>
-    <mergeCell ref="BK9:BL9"/>
-    <mergeCell ref="BO9:BP9"/>
-    <mergeCell ref="BQ9:BR9"/>
-    <mergeCell ref="AK9:AL9"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="S9:T9"/>
-    <mergeCell ref="U9:V9"/>
-    <mergeCell ref="Y9:Z9"/>
-    <mergeCell ref="AA9:AB9"/>
-    <mergeCell ref="AE9:AF9"/>
-    <mergeCell ref="AG9:AH9"/>
-    <mergeCell ref="AS8:AX8"/>
-    <mergeCell ref="AY8:BD8"/>
-    <mergeCell ref="BE8:BJ8"/>
-    <mergeCell ref="BK8:BP8"/>
-    <mergeCell ref="BQ8:BV8"/>
-    <mergeCell ref="G15:P15"/>
-    <mergeCell ref="AG8:AL8"/>
-    <mergeCell ref="AW6:BD6"/>
-    <mergeCell ref="AA6:AF6"/>
-    <mergeCell ref="CI3:CT3"/>
-    <mergeCell ref="C3:H3"/>
-    <mergeCell ref="C8:H8"/>
-    <mergeCell ref="I8:N8"/>
-    <mergeCell ref="O8:T8"/>
-    <mergeCell ref="U8:Z8"/>
-    <mergeCell ref="AA8:AF8"/>
-    <mergeCell ref="BW8:CB8"/>
-    <mergeCell ref="CC8:CH8"/>
-    <mergeCell ref="CI8:CN8"/>
-    <mergeCell ref="CO8:CT8"/>
-    <mergeCell ref="AM8:AR8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" scale="74" fitToWidth="0" orientation="landscape" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>